<commit_message>
factor out cumulant scaling
</commit_message>
<xml_diff>
--- a/tblack.xlsx
+++ b/tblack.xlsx
@@ -12,15 +12,26 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="6825"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BLACK" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Delta">BLACK!$C$9</definedName>
+    <definedName name="epsilon">BLACK!$C$2</definedName>
+    <definedName name="Expiration" localSheetId="0">BLACK!$C$7</definedName>
     <definedName name="expiration">Sheet1!$E$3</definedName>
+    <definedName name="Forward" localSheetId="0">BLACK!$C$4</definedName>
     <definedName name="forward">Sheet1!$B$3</definedName>
+    <definedName name="Gamma">BLACK!$C$10</definedName>
     <definedName name="iforward">Sheet1!$H$3</definedName>
     <definedName name="ivolatility">Sheet1!$G$3</definedName>
+    <definedName name="Strike" localSheetId="0">BLACK!$C$6</definedName>
     <definedName name="strike">Sheet1!$D$3</definedName>
+    <definedName name="Theta">BLACK!$C$12</definedName>
+    <definedName name="Value" localSheetId="0">BLACK!$C$8</definedName>
     <definedName name="value">Sheet1!$F$3</definedName>
+    <definedName name="Vega">BLACK!$C$11</definedName>
+    <definedName name="Volatility" localSheetId="0">BLACK!$C$5</definedName>
     <definedName name="volatility">Sheet1!$C$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -33,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>forward</t>
   </si>
@@ -55,12 +66,51 @@
   <si>
     <t>ivolatility</t>
   </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Volatility</t>
+  </si>
+  <si>
+    <t>Strike</t>
+  </si>
+  <si>
+    <t>Expiration</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Vega</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>epsilon</t>
+  </si>
+  <si>
+    <t>approx</t>
+  </si>
+  <si>
+    <t>abs</t>
+  </si>
+  <si>
+    <t>rel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +118,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -85,15 +189,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="1" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -371,11 +567,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <f>Forward+epsilon</f>
+        <v>100.000001</v>
+      </c>
+      <c r="F4">
+        <f>Forward - epsilon</f>
+        <v>99.999999000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G5">
+        <f>Volatility + epsilon</f>
+        <v>0.20000100000000001</v>
+      </c>
+      <c r="H5">
+        <f>Volatility - epsilon</f>
+        <v>0.19999900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="I7">
+        <f>Expiration+epsilon</f>
+        <v>0.25000099999999997</v>
+      </c>
+      <c r="J7">
+        <f>Expiration-epsilon</f>
+        <v>0.249999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="array" ref="C8:C12">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, Expiration)</f>
+        <v>3.987761167674492</v>
+      </c>
+      <c r="D8" s="5">
+        <f>Value-_xll.XLL.BLACK.VALUE(Forward, Volatility, Strike, Expiration)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="array" ref="E8:E12">_xll.XLL.BLACK.GREEKS(E4, Volatility, Strike, Expiration)</f>
+        <v>3.9877616876133217</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="array" ref="F8:F12">_xll.XLL.BLACK.GREEKS(F4, Volatility, Strike, Expiration)</f>
+        <v>3.9877606477357119</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="array" ref="G8:G12">_xll.XLL.BLACK.GREEKS(Forward, G5, Strike, Expiration)</f>
+        <v>3.9877810898700758</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="array" ref="H8:H12">_xll.XLL.BLACK.GREEKS(Forward, H5, Strike, Expiration)</f>
+        <v>3.9877412454786665</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="array" ref="I8:I12">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, I7)</f>
+        <v>3.9877691365447916</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="array" ref="J8:J12">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, J7)</f>
+        <v>3.9877531987882193</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.51993880583837249</v>
+      </c>
+      <c r="D9" s="5">
+        <f>Delta-_xll.XLL.BLACK.DELTA(Forward, Volatility, Strike, Expiration)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.51993884568276338</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.51993876599398103</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.5199389054493504</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.51993870622739335</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.51993884568272397</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.51993876599394107</v>
+      </c>
+      <c r="K9">
+        <f>(E8-F8)/(E4-F4)</f>
+        <v>0.5199388062120307</v>
+      </c>
+      <c r="L9" s="5">
+        <f>Delta-K9</f>
+        <v>-3.7365821548007716E-10</v>
+      </c>
+      <c r="M9" s="5">
+        <f>L9/Delta</f>
+        <v>-7.1865806376497327E-10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3.9844391409476397E-2</v>
+      </c>
+      <c r="D10" s="5">
+        <f>Gamma-_xll.XLL.BLACK.GAMMA(Forward, Volatility, Strike, Expiration)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3.9844390811810328E-2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3.9844392007142071E-2</v>
+      </c>
+      <c r="G10" s="7">
+        <v>3.9844191690461814E-2</v>
+      </c>
+      <c r="H10" s="7">
+        <v>3.9844591130485697E-2</v>
+      </c>
+      <c r="I10" s="7">
+        <v>3.9844311521711084E-2</v>
+      </c>
+      <c r="J10" s="7">
+        <v>3.9844471297720632E-2</v>
+      </c>
+      <c r="K10">
+        <f>(E8-2*Value+F8)/(epsilon^2)</f>
+        <v>4.9737991503207013E-2</v>
+      </c>
+      <c r="L10" s="5">
+        <f>Gamma-K10</f>
+        <v>-9.8936000937306159E-3</v>
+      </c>
+      <c r="M10" s="5">
+        <f>L10/Gamma</f>
+        <v>-0.24830596587748532</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6">
+        <v>19.922195704738197</v>
+      </c>
+      <c r="D11" s="5">
+        <f>Vega-_xll.XLL.BLACK.VEGA(Forward, Volatility, Strike, Expiration)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>19.92219580434908</v>
+      </c>
+      <c r="F11" s="7">
+        <v>19.922195605127119</v>
+      </c>
+      <c r="G11" s="7">
+        <v>19.922195455710131</v>
+      </c>
+      <c r="H11" s="7">
+        <v>19.922195953765023</v>
+      </c>
+      <c r="I11" s="7">
+        <v>19.922235449478581</v>
+      </c>
+      <c r="J11" s="7">
+        <v>19.922155959917724</v>
+      </c>
+      <c r="K11">
+        <f>(G8-H8)/(G5-H5)</f>
+        <v>19.922195704660311</v>
+      </c>
+      <c r="L11" s="5">
+        <f>Vega-K11</f>
+        <v>7.7886141980343382E-11</v>
+      </c>
+      <c r="M11" s="5">
+        <f>L11/Vega</f>
+        <v>3.9095159557045875E-12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-7.9688782818952797</v>
+      </c>
+      <c r="D12" s="5">
+        <f>Theta-_xll.XLL.BLACK.THETA(Forward, Volatility, Strike, Expiration)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>-7.9688783217396324</v>
+      </c>
+      <c r="F12" s="7">
+        <v>-7.9688782420508479</v>
+      </c>
+      <c r="G12" s="7">
+        <v>-7.968918026674964</v>
+      </c>
+      <c r="H12" s="7">
+        <v>-7.9688385371141015</v>
+      </c>
+      <c r="I12" s="7">
+        <v>-7.9688623043422169</v>
+      </c>
+      <c r="J12" s="7">
+        <v>-7.9688942595441281</v>
+      </c>
+      <c r="K12">
+        <f>-(I8-J8)/(I7-J7)</f>
+        <v>-7.9688782862379712</v>
+      </c>
+      <c r="L12" s="5">
+        <f>Theta-K12</f>
+        <v>4.3426915397049015E-9</v>
+      </c>
+      <c r="M12" s="5">
+        <f>L12/Theta</f>
+        <v>-5.4495644005144175E-10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -415,13 +907,13 @@
       <c r="E3">
         <v>0.25</v>
       </c>
-      <c r="F3">
-        <f>_xll.BLACK.VALUE(forward, volatility, strike, expiration)</f>
-        <v>0.19947093241844982</v>
-      </c>
-      <c r="G3">
-        <f>_xll.BLACK.IMPLIED.VOLATILITY(forward, value, strike, expiration)</f>
-        <v>9.9999999999990756E-3</v>
+      <c r="F3" t="e">
+        <f ca="1">_xll.BLACK.VALUE(forward, volatility, strike, expiration)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G3" t="e">
+        <f ca="1">_xll.BLACK.IMPLIED.VOLATILITY(forward, value, strike, expiration)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
improved guess for initial vol in black::implied
</commit_message>
<xml_diff>
--- a/tblack.xlsx
+++ b/tblack.xlsx
@@ -14,24 +14,30 @@
   <sheets>
     <sheet name="BLACK" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="IMPLIED.VOLATILITY" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Delta">BLACK!$C$9</definedName>
     <definedName name="epsilon">BLACK!$C$2</definedName>
     <definedName name="Expiration" localSheetId="0">BLACK!$C$7</definedName>
+    <definedName name="Expiration" localSheetId="2">IMPLIED.VOLATILITY!$C$5</definedName>
     <definedName name="expiration">Sheet1!$E$3</definedName>
     <definedName name="Forward" localSheetId="0">BLACK!$C$4</definedName>
+    <definedName name="Forward" localSheetId="2">IMPLIED.VOLATILITY!$C$2</definedName>
     <definedName name="forward">Sheet1!$B$3</definedName>
     <definedName name="Gamma">BLACK!$C$10</definedName>
     <definedName name="iforward">Sheet1!$H$3</definedName>
     <definedName name="ivolatility">Sheet1!$G$3</definedName>
     <definedName name="Strike" localSheetId="0">BLACK!$C$6</definedName>
+    <definedName name="Strike" localSheetId="2">IMPLIED.VOLATILITY!$C$4</definedName>
     <definedName name="strike">Sheet1!$D$3</definedName>
     <definedName name="Theta">BLACK!$C$12</definedName>
     <definedName name="Value" localSheetId="0">BLACK!$C$8</definedName>
+    <definedName name="Value" localSheetId="2">IMPLIED.VOLATILITY!$C$6</definedName>
     <definedName name="value">Sheet1!$F$3</definedName>
     <definedName name="Vega">BLACK!$C$11</definedName>
     <definedName name="Volatility" localSheetId="0">BLACK!$C$5</definedName>
+    <definedName name="Volatility" localSheetId="2">IMPLIED.VOLATILITY!$C$3</definedName>
     <definedName name="volatility">Sheet1!$C$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -44,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>forward</t>
   </si>
@@ -104,6 +110,9 @@
   </si>
   <si>
     <t>rel</t>
+  </si>
+  <si>
+    <t>Implied</t>
   </si>
 </sst>
 </file>
@@ -268,7 +277,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -283,6 +292,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -567,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M12"/>
+  <dimension ref="B2:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,9 +595,17 @@
         <v>16</v>
       </c>
       <c r="C2" s="3">
-        <v>9.9999999999999995E-7</v>
+        <v>1E-4</v>
       </c>
       <c r="D2" s="3"/>
+      <c r="E2">
+        <f>E4-Forward</f>
+        <v>1.0000000000331966E-4</v>
+      </c>
+      <c r="F2">
+        <f>F4-Forward</f>
+        <v>-1.0000000000331966E-4</v>
+      </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -596,11 +616,11 @@
       </c>
       <c r="E4">
         <f>Forward+epsilon</f>
-        <v>100.000001</v>
+        <v>100.0001</v>
       </c>
       <c r="F4">
         <f>Forward - epsilon</f>
-        <v>99.999999000000003</v>
+        <v>99.999899999999997</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -612,11 +632,11 @@
       </c>
       <c r="G5">
         <f>Volatility + epsilon</f>
-        <v>0.20000100000000001</v>
+        <v>0.2001</v>
       </c>
       <c r="H5">
         <f>Volatility - epsilon</f>
-        <v>0.19999900000000001</v>
+        <v>0.19990000000000002</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -624,7 +644,8 @@
         <v>9</v>
       </c>
       <c r="C6" s="4">
-        <v>100</v>
+        <f ca="1">100 + INT(100*RAND()) - 50</f>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -636,11 +657,11 @@
       </c>
       <c r="I7">
         <f>Expiration+epsilon</f>
-        <v>0.25000099999999997</v>
+        <v>0.25009999999999999</v>
       </c>
       <c r="J7">
         <f>Expiration-epsilon</f>
-        <v>0.249999</v>
+        <v>0.24990000000000001</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -648,36 +669,36 @@
         <v>11</v>
       </c>
       <c r="C8" s="8">
-        <f t="array" ref="C8:C12">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, Expiration)</f>
-        <v>3.987761167674492</v>
+        <f t="array" aca="1" ref="C8:C12" ca="1">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, Expiration)</f>
+        <v>18.080058534547859</v>
       </c>
       <c r="D8" s="5">
-        <f>Value-_xll.XLL.BLACK.VALUE(Forward, Volatility, Strike, Expiration)</f>
+        <f ca="1">Value-_xll.XLL.BLACK.VALUE(Forward, Volatility, Strike, Expiration)</f>
         <v>0</v>
       </c>
       <c r="E8" s="9">
-        <f t="array" ref="E8:E12">_xll.XLL.BLACK.GREEKS(E4, Volatility, Strike, Expiration)</f>
-        <v>3.9877616876133217</v>
+        <f t="array" aca="1" ref="E8:E12" ca="1">_xll.XLL.BLACK.GREEKS(E4, Volatility, Strike, Expiration)</f>
+        <v>18.080156439559914</v>
       </c>
       <c r="F8" s="7">
-        <f t="array" ref="F8:F12">_xll.XLL.BLACK.GREEKS(F4, Volatility, Strike, Expiration)</f>
-        <v>3.9877606477357119</v>
+        <f t="array" aca="1" ref="F8:F12" ca="1">_xll.XLL.BLACK.GREEKS(F4, Volatility, Strike, Expiration)</f>
+        <v>18.079960629586211</v>
       </c>
       <c r="G8" s="7">
-        <f t="array" ref="G8:G12">_xll.XLL.BLACK.GREEKS(Forward, G5, Strike, Expiration)</f>
-        <v>3.9877810898700758</v>
+        <f t="array" aca="1" ref="G8:G12" ca="1">_xll.XLL.BLACK.GREEKS(Forward, G5, Strike, Expiration)</f>
+        <v>18.080310583682774</v>
       </c>
       <c r="H8" s="7">
-        <f t="array" ref="H8:H12">_xll.XLL.BLACK.GREEKS(Forward, H5, Strike, Expiration)</f>
-        <v>3.9877412454786665</v>
+        <f t="array" aca="1" ref="H8:H12" ca="1">_xll.XLL.BLACK.GREEKS(Forward, H5, Strike, Expiration)</f>
+        <v>18.079806980929945</v>
       </c>
       <c r="I8" s="7">
-        <f t="array" ref="I8:I12">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, I7)</f>
-        <v>3.9877691365447916</v>
+        <f t="array" aca="1" ref="I8:I12" ca="1">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, I7)</f>
+        <v>18.080159284648872</v>
       </c>
       <c r="J8" s="7">
-        <f t="array" ref="J8:J12">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, J7)</f>
-        <v>3.9877531987882193</v>
+        <f t="array" aca="1" ref="J8:J12" ca="1">_xll.XLL.BLACK.GREEKS(Forward, Volatility, Strike, J7)</f>
+        <v>18.079957843585476</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>17</v>
@@ -694,41 +715,48 @@
         <v>12</v>
       </c>
       <c r="C9" s="6">
-        <v>0.51993880583837249</v>
+        <f ca="1"/>
+        <v>0.97904986844764075</v>
       </c>
       <c r="D9" s="5">
-        <f>Delta-_xll.XLL.BLACK.DELTA(Forward, Volatility, Strike, Expiration)</f>
+        <f ca="1">Delta-_xll.XLL.BLACK.DELTA(Forward, Volatility, Strike, Expiration)</f>
         <v>0</v>
       </c>
       <c r="E9" s="7">
-        <v>0.51993884568276338</v>
+        <f ca="1"/>
+        <v>0.97905037204494194</v>
       </c>
       <c r="F9" s="7">
-        <v>0.51993876599398103</v>
+        <f ca="1"/>
+        <v>0.97904936483959026</v>
       </c>
       <c r="G9" s="7">
-        <v>0.5199389054493504</v>
+        <f ca="1"/>
+        <v>0.97900113431127966</v>
       </c>
       <c r="H9" s="7">
-        <v>0.51993870622739335</v>
+        <f ca="1"/>
+        <v>0.979098556695984</v>
       </c>
       <c r="I9" s="7">
-        <v>0.51993884568272397</v>
+        <f ca="1"/>
+        <v>0.9790303822441393</v>
       </c>
       <c r="J9" s="7">
-        <v>0.51993876599394107</v>
+        <f ca="1"/>
+        <v>0.97906935120595451</v>
       </c>
       <c r="K9">
-        <f>(E8-F8)/(E4-F4)</f>
-        <v>0.5199388062120307</v>
+        <f ca="1">(E8-F8)/(E4-F4)</f>
+        <v>0.97904986848665398</v>
       </c>
       <c r="L9" s="5">
-        <f>Delta-K9</f>
-        <v>-3.7365821548007716E-10</v>
+        <f ca="1">Delta-K9</f>
+        <v>-3.9013237085328001E-11</v>
       </c>
       <c r="M9" s="5">
-        <f>L9/Delta</f>
-        <v>-7.1865806376497327E-10</v>
+        <f ca="1">L9/Delta</f>
+        <v>-3.9848059166982479E-11</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -736,41 +764,48 @@
         <v>13</v>
       </c>
       <c r="C10" s="6">
-        <v>3.9844391409476397E-2</v>
+        <f ca="1"/>
+        <v>5.0360267574508771E-3</v>
       </c>
       <c r="D10" s="5">
-        <f>Gamma-_xll.XLL.BLACK.GAMMA(Forward, Volatility, Strike, Expiration)</f>
+        <f ca="1">Gamma-_xll.XLL.BLACK.GAMMA(Forward, Volatility, Strike, Expiration)</f>
         <v>0</v>
       </c>
       <c r="E10" s="7">
-        <v>3.9844390811810328E-2</v>
+        <f ca="1"/>
+        <v>5.035919263936167E-3</v>
       </c>
       <c r="F10" s="7">
-        <v>3.9844392007142071E-2</v>
+        <f ca="1"/>
+        <v>5.0361342528639523E-3</v>
       </c>
       <c r="G10" s="7">
-        <v>3.9844191690461814E-2</v>
+        <f ca="1"/>
+        <v>5.0434176979126562E-3</v>
       </c>
       <c r="H10" s="7">
-        <v>3.9844591130485697E-2</v>
+        <f ca="1"/>
+        <v>5.0286330490132026E-3</v>
       </c>
       <c r="I10" s="7">
-        <v>3.9844311521711084E-2</v>
+        <f ca="1"/>
+        <v>5.0389831710738395E-3</v>
       </c>
       <c r="J10" s="7">
-        <v>3.9844471297720632E-2</v>
+        <f ca="1"/>
+        <v>5.0330693095650648E-3</v>
       </c>
       <c r="K10">
-        <f>(E8-2*Value+F8)/(epsilon^2)</f>
-        <v>4.9737991503207013E-2</v>
+        <f ca="1">(E8-2*Value+F8)/(epsilon^2)</f>
+        <v>5.0405901674821507E-3</v>
       </c>
       <c r="L10" s="5">
-        <f>Gamma-K10</f>
-        <v>-9.8936000937306159E-3</v>
+        <f ca="1">Gamma-K10</f>
+        <v>-4.5634100312736542E-6</v>
       </c>
       <c r="M10" s="5">
-        <f>L10/Gamma</f>
-        <v>-0.24830596587748532</v>
+        <f ca="1">L10/Gamma</f>
+        <v>-9.0615285642039545E-4</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -778,41 +813,48 @@
         <v>14</v>
       </c>
       <c r="C11" s="6">
-        <v>19.922195704738197</v>
+        <f ca="1"/>
+        <v>2.5180133787254388</v>
       </c>
       <c r="D11" s="5">
-        <f>Vega-_xll.XLL.BLACK.VEGA(Forward, Volatility, Strike, Expiration)</f>
+        <f ca="1">Vega-_xll.XLL.BLACK.VEGA(Forward, Volatility, Strike, Expiration)</f>
         <v>0</v>
       </c>
       <c r="E11" s="7">
-        <v>19.92219580434908</v>
+        <f ca="1"/>
+        <v>2.5179646678898657</v>
       </c>
       <c r="F11" s="7">
-        <v>19.922195605127119</v>
+        <f ca="1"/>
+        <v>2.5180620903002415</v>
       </c>
       <c r="G11" s="7">
-        <v>19.922195455710131</v>
+        <f ca="1"/>
+        <v>2.5229697033808072</v>
       </c>
       <c r="H11" s="7">
-        <v>19.922195953765023</v>
+        <f ca="1"/>
+        <v>2.5130593662443479</v>
       </c>
       <c r="I11" s="7">
-        <v>19.922235449478581</v>
+        <f ca="1"/>
+        <v>2.5204993821711343</v>
       </c>
       <c r="J11" s="7">
-        <v>19.922155959917724</v>
+        <f ca="1"/>
+        <v>2.5155280409206191</v>
       </c>
       <c r="K11">
-        <f>(G8-H8)/(G5-H5)</f>
-        <v>19.922195704660311</v>
+        <f ca="1">(G8-H8)/(G5-H5)</f>
+        <v>2.5180137641458984</v>
       </c>
       <c r="L11" s="5">
-        <f>Vega-K11</f>
-        <v>7.7886141980343382E-11</v>
+        <f ca="1">Vega-K11</f>
+        <v>-3.8542045954770288E-7</v>
       </c>
       <c r="M11" s="5">
-        <f>L11/Vega</f>
-        <v>3.9095159557045875E-12</v>
+        <f ca="1">L11/Vega</f>
+        <v>-1.5306529457075164E-7</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -820,41 +862,57 @@
         <v>15</v>
       </c>
       <c r="C12" s="6">
-        <v>-7.9688782818952797</v>
+        <f ca="1"/>
+        <v>-1.0072053514901755</v>
       </c>
       <c r="D12" s="5">
-        <f>Theta-_xll.XLL.BLACK.THETA(Forward, Volatility, Strike, Expiration)</f>
+        <f ca="1">Theta-_xll.XLL.BLACK.THETA(Forward, Volatility, Strike, Expiration)</f>
         <v>0</v>
       </c>
       <c r="E12" s="7">
-        <v>-7.9688783217396324</v>
+        <f ca="1"/>
+        <v>-1.0071858671559464</v>
       </c>
       <c r="F12" s="7">
-        <v>-7.9688782420508479</v>
+        <f ca="1"/>
+        <v>-1.0072248361200966</v>
       </c>
       <c r="G12" s="7">
-        <v>-7.968918026674964</v>
+        <f ca="1"/>
+        <v>-1.009692475292999</v>
       </c>
       <c r="H12" s="7">
-        <v>-7.9688385371141015</v>
+        <f ca="1"/>
+        <v>-1.0047211346244904</v>
       </c>
       <c r="I12" s="7">
-        <v>-7.9688623043422169</v>
+        <f ca="1"/>
+        <v>-1.007796634214768</v>
       </c>
       <c r="J12" s="7">
-        <v>-7.9688942595441281</v>
+        <f ca="1"/>
+        <v>-1.0066138619130129</v>
       </c>
       <c r="K12">
-        <f>-(I8-J8)/(I7-J7)</f>
-        <v>-7.9688782862379712</v>
+        <f ca="1">-(I8-J8)/(I7-J7)</f>
+        <v>-1.0072053169808415</v>
       </c>
       <c r="L12" s="5">
-        <f>Theta-K12</f>
-        <v>4.3426915397049015E-9</v>
+        <f ca="1">Theta-K12</f>
+        <v>-3.4509334057020169E-8</v>
       </c>
       <c r="M12" s="5">
-        <f>L12/Theta</f>
-        <v>-5.4495644005144175E-10</v>
+        <f ca="1">L12/Theta</f>
+        <v>3.426246098272124E-8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="e">
+        <f ca="1">_xll.XLL.BLACK.IMPLIED.VOLATILITY(Forward, Value, Strike, Expiration)</f>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
@@ -867,7 +925,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H202"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -907,13 +967,13 @@
       <c r="E3">
         <v>0.25</v>
       </c>
-      <c r="F3" t="e">
-        <f ca="1">_xll.BLACK.VALUE(forward, volatility, strike, expiration)</f>
-        <v>#NAME?</v>
+      <c r="F3">
+        <f>_xll.XLL.BLACK.VALUE(B3,C3,D3,E3)</f>
+        <v>0.19947093241847824</v>
       </c>
       <c r="G3" t="e">
-        <f ca="1">_xll.BLACK.IMPLIED.VOLATILITY(forward, value, strike, expiration)</f>
-        <v>#NAME?</v>
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B3, F3, D3, E3)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -930,8 +990,12 @@
         <v>0.25</v>
       </c>
       <c r="F4">
-        <f>_xll.BLACK.VALUE(B4,C4,D4,E4)</f>
-        <v>0.39894061814813142</v>
+        <f>_xll.XLL.BLACK.VALUE(B4,C4,D4,E4)</f>
+        <v>0.39894061814816695</v>
+      </c>
+      <c r="G4" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B4, F4, D4, E4)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -948,8 +1012,12 @@
         <v>0.25</v>
       </c>
       <c r="F5">
-        <f>_xll.BLACK.VALUE(B5,C5,D5,E5)</f>
+        <f>_xll.XLL.BLACK.VALUE(B5,C5,D5,E5)</f>
         <v>0.59840781052366765</v>
+      </c>
+      <c r="G5" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B5, F5, D5, E5)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -966,8 +1034,12 @@
         <v>0.25</v>
       </c>
       <c r="F6">
-        <f>_xll.BLACK.VALUE(B6,C6,D6,E6)</f>
+        <f>_xll.XLL.BLACK.VALUE(B6,C6,D6,E6)</f>
         <v>0.79787126292632138</v>
+      </c>
+      <c r="G6" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B6, F6, D6, E6)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -984,8 +1056,12 @@
         <v>0.25</v>
       </c>
       <c r="F7">
-        <f>_xll.BLACK.VALUE(B7,C7,D7,E7)</f>
+        <f>_xll.XLL.BLACK.VALUE(B7,C7,D7,E7)</f>
         <v>0.99732972880759974</v>
+      </c>
+      <c r="G7" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B7, F7, D7, E7)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1002,8 +1078,12 @@
         <v>0.25</v>
       </c>
       <c r="F8">
-        <f>_xll.BLACK.VALUE(B8,C8,D8,E8)</f>
-        <v>1.1967819617124746</v>
+        <f>_xll.XLL.BLACK.VALUE(B8,C8,D8,E8)</f>
+        <v>1.1967819617124462</v>
+      </c>
+      <c r="G8" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B8, F8, D8, E8)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -1020,8 +1100,12 @@
         <v>0.25</v>
       </c>
       <c r="F9">
-        <f>_xll.BLACK.VALUE(B9,C9,D9,E9)</f>
-        <v>1.3962267153027028</v>
+        <f>_xll.XLL.BLACK.VALUE(B9,C9,D9,E9)</f>
+        <v>1.3962267153026957</v>
+      </c>
+      <c r="G9" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B9, F9, D9, E9)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1038,8 +1122,12 @@
         <v>0.25</v>
       </c>
       <c r="F10">
-        <f>_xll.BLACK.VALUE(B10,C10,D10,E10)</f>
-        <v>1.5956627433803874</v>
+        <f>_xll.XLL.BLACK.VALUE(B10,C10,D10,E10)</f>
+        <v>1.5956627433803945</v>
+      </c>
+      <c r="G10" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B10, F10, D10, E10)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1056,8 +1144,12 @@
         <v>0.25</v>
       </c>
       <c r="F11">
-        <f>_xll.BLACK.VALUE(B11,C11,D11,E11)</f>
+        <f>_xll.XLL.BLACK.VALUE(B11,C11,D11,E11)</f>
         <v>1.79508879991117</v>
+      </c>
+      <c r="G11" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B11, F11, D11, E11)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -1074,8 +1166,12 @@
         <v>0.25</v>
       </c>
       <c r="F12">
-        <f>_xll.BLACK.VALUE(B12,C12,D12,E12)</f>
-        <v>1.9945036390475792</v>
+        <f>_xll.XLL.BLACK.VALUE(B12,C12,D12,E12)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="G12" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B12, F12, D12, E12)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1092,8 +1188,12 @@
         <v>0.25</v>
       </c>
       <c r="F13">
-        <f>_xll.BLACK.VALUE(B13,C13,D13,E13)</f>
+        <f>_xll.XLL.BLACK.VALUE(B13,C13,D13,E13)</f>
         <v>2.1939060151525638</v>
+      </c>
+      <c r="G13" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B13, F13, D13, E13)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1110,8 +1210,12 @@
         <v>0.25</v>
       </c>
       <c r="F14">
-        <f>_xll.BLACK.VALUE(B14,C14,D14,E14)</f>
-        <v>2.3932946828224999</v>
+        <f>_xll.XLL.BLACK.VALUE(B14,C14,D14,E14)</f>
+        <v>2.3932946828225283</v>
+      </c>
+      <c r="G14" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B14, F14, D14, E14)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1128,8 +1232,12 @@
         <v>0.25</v>
       </c>
       <c r="F15">
-        <f>_xll.BLACK.VALUE(B15,C15,D15,E15)</f>
-        <v>2.5926683969109519</v>
+        <f>_xll.XLL.BLACK.VALUE(B15,C15,D15,E15)</f>
+        <v>2.5926683969109732</v>
+      </c>
+      <c r="G15" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B15, F15, D15, E15)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1146,11 +1254,15 @@
         <v>0.25</v>
       </c>
       <c r="F16">
-        <f>_xll.BLACK.VALUE(B16,C16,D16,E16)</f>
-        <v>2.7920259125516509</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B16,C16,D16,E16)</f>
+        <v>2.792025912551658</v>
+      </c>
+      <c r="G16" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B16, F16, D16, E16)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>100</v>
       </c>
@@ -1164,11 +1276,15 @@
         <v>0.25</v>
       </c>
       <c r="F17">
-        <f>_xll.BLACK.VALUE(B17,C17,D17,E17)</f>
-        <v>2.991365985181929</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B17,C17,D17,E17)</f>
+        <v>2.9913659851819503</v>
+      </c>
+      <c r="G17" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B17, F17, D17, E17)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>100</v>
       </c>
@@ -1182,11 +1298,15 @@
         <v>0.25</v>
       </c>
       <c r="F18">
-        <f>_xll.BLACK.VALUE(B18,C18,D18,E18)</f>
-        <v>3.1906873705661098</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B18,C18,D18,E18)</f>
+        <v>3.1906873705661525</v>
+      </c>
+      <c r="G18" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B18, F18, D18, E18)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>100</v>
       </c>
@@ -1200,11 +1320,15 @@
         <v>0.25</v>
       </c>
       <c r="F19">
-        <f>_xll.BLACK.VALUE(B19,C19,D19,E19)</f>
-        <v>3.389988824818829</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B19,C19,D19,E19)</f>
+        <v>3.3899888248187651</v>
+      </c>
+      <c r="G19" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B19, F19, D19, E19)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>100</v>
       </c>
@@ -1218,11 +1342,15 @@
         <v>0.25</v>
       </c>
       <c r="F20">
-        <f>_xll.BLACK.VALUE(B20,C20,D20,E20)</f>
-        <v>3.589269104427828</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B20,C20,D20,E20)</f>
+        <v>3.5892691044278067</v>
+      </c>
+      <c r="G20" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B20, F20, D20, E20)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>100</v>
       </c>
@@ -1236,11 +1364,15 @@
         <v>0.25</v>
       </c>
       <c r="F21">
-        <f>_xll.BLACK.VALUE(B21,C21,D21,E21)</f>
-        <v>3.7885269662780701</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B21,C21,D21,E21)</f>
+        <v>3.7885269662781056</v>
+      </c>
+      <c r="G21" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B21, F21, D21, E21)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>100</v>
       </c>
@@ -1254,11 +1386,15 @@
         <v>0.25</v>
       </c>
       <c r="F22">
-        <f>_xll.BLACK.VALUE(B22,C22,D22,E22)</f>
-        <v>3.9877611676745346</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B22,C22,D22,E22)</f>
+        <v>3.987761167674492</v>
+      </c>
+      <c r="G22" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B22, F22, D22, E22)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>100</v>
       </c>
@@ -1272,11 +1408,15 @@
         <v>0.25</v>
       </c>
       <c r="F23">
-        <f>_xll.BLACK.VALUE(B23,C23,D23,E23)</f>
-        <v>4.1869704663651532</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B23,C23,D23,E23)</f>
+        <v>4.1869704663651319</v>
+      </c>
+      <c r="G23" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B23, F23, D23, E23)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>100</v>
       </c>
@@ -1290,11 +1430,15 @@
         <v>0.25</v>
       </c>
       <c r="F24">
-        <f>_xll.BLACK.VALUE(B24,C24,D24,E24)</f>
-        <v>4.3861536205646701</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B24,C24,D24,E24)</f>
+        <v>4.3861536205646985</v>
+      </c>
+      <c r="G24" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B24, F24, D24, E24)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>100</v>
       </c>
@@ -1308,11 +1452,15 @@
         <v>0.25</v>
       </c>
       <c r="F25">
-        <f>_xll.BLACK.VALUE(B25,C25,D25,E25)</f>
-        <v>4.585309388977592</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B25,C25,D25,E25)</f>
+        <v>4.5853093889776417</v>
+      </c>
+      <c r="G25" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B25, F25, D25, E25)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>100</v>
       </c>
@@ -1326,11 +1474,15 @@
         <v>0.25</v>
       </c>
       <c r="F26">
-        <f>_xll.BLACK.VALUE(B26,C26,D26,E26)</f>
-        <v>4.7844365308213526</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B26,C26,D26,E26)</f>
+        <v>4.7844365308213668</v>
+      </c>
+      <c r="G26" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B26, F26, D26, E26)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>100</v>
       </c>
@@ -1344,11 +1496,15 @@
         <v>0.25</v>
       </c>
       <c r="F27">
-        <f>_xll.BLACK.VALUE(B27,C27,D27,E27)</f>
-        <v>4.9835338058494614</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B27,C27,D27,E27)</f>
+        <v>4.9835338058494401</v>
+      </c>
+      <c r="G27" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B27, F27, D27, E27)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>100</v>
       </c>
@@ -1362,11 +1518,15 @@
         <v>0.25</v>
       </c>
       <c r="F28">
-        <f>_xll.BLACK.VALUE(B28,C28,D28,E28)</f>
-        <v>5.1825999743747388</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B28,C28,D28,E28)</f>
+        <v>5.1825999743747531</v>
+      </c>
+      <c r="G28" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B28, F28, D28, E28)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>100</v>
       </c>
@@ -1380,11 +1540,15 @@
         <v>0.25</v>
       </c>
       <c r="F29">
-        <f>_xll.BLACK.VALUE(B29,C29,D29,E29)</f>
+        <f>_xll.XLL.BLACK.VALUE(B29,C29,D29,E29)</f>
         <v>5.3816337972926789</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B29, F29, D29, E29)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>100</v>
       </c>
@@ -1398,11 +1562,15 @@
         <v>0.25</v>
       </c>
       <c r="F30">
-        <f>_xll.BLACK.VALUE(B30,C30,D30,E30)</f>
-        <v>5.580634036104243</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B30,C30,D30,E30)</f>
+        <v>5.5806340361042288</v>
+      </c>
+      <c r="G30" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B30, F30, D30, E30)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>100</v>
       </c>
@@ -1416,11 +1584,15 @@
         <v>0.25</v>
       </c>
       <c r="F31">
-        <f>_xll.BLACK.VALUE(B31,C31,D31,E31)</f>
-        <v>5.7795994529390384</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B31,C31,D31,E31)</f>
+        <v>5.7795994529391095</v>
+      </c>
+      <c r="G31" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B31, F31, D31, E31)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>100</v>
       </c>
@@ -1434,11 +1606,15 @@
         <v>0.25</v>
       </c>
       <c r="F32">
-        <f>_xll.BLACK.VALUE(B32,C32,D32,E32)</f>
-        <v>5.9785288105789931</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B32,C32,D32,E32)</f>
+        <v>5.9785288105789576</v>
+      </c>
+      <c r="G32" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B32, F32, D32, E32)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>100</v>
       </c>
@@ -1452,11 +1628,15 @@
         <v>0.25</v>
       </c>
       <c r="F33">
-        <f>_xll.BLACK.VALUE(B33,C33,D33,E33)</f>
-        <v>6.1774208724802264</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B33,C33,D33,E33)</f>
+        <v>6.1774208724802335</v>
+      </c>
+      <c r="G33" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B33, F33, D33, E33)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>100</v>
       </c>
@@ -1470,11 +1650,15 @@
         <v>0.25</v>
       </c>
       <c r="F34">
-        <f>_xll.BLACK.VALUE(B34,C34,D34,E34)</f>
-        <v>6.3762744027974918</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B34,C34,D34,E34)</f>
+        <v>6.3762744027974705</v>
+      </c>
+      <c r="G34" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B34, F34, D34, E34)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>100</v>
       </c>
@@ -1488,11 +1672,15 @@
         <v>0.25</v>
       </c>
       <c r="F35">
-        <f>_xll.BLACK.VALUE(B35,C35,D35,E35)</f>
-        <v>6.5750881664062177</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B35,C35,D35,E35)</f>
+        <v>6.5750881664061538</v>
+      </c>
+      <c r="G35" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B35, F35, D35, E35)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>100</v>
       </c>
@@ -1506,11 +1694,15 @@
         <v>0.25</v>
       </c>
       <c r="F36">
-        <f>_xll.BLACK.VALUE(B36,C36,D36,E36)</f>
-        <v>6.773860928925842</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B36,C36,D36,E36)</f>
+        <v>6.7738609289258349</v>
+      </c>
+      <c r="G36" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B36, F36, D36, E36)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>100</v>
       </c>
@@ -1524,11 +1716,15 @@
         <v>0.25</v>
       </c>
       <c r="F37">
-        <f>_xll.BLACK.VALUE(B37,C37,D37,E37)</f>
+        <f>_xll.XLL.BLACK.VALUE(B37,C37,D37,E37)</f>
         <v>6.9725914567430749</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B37, F37, D37, E37)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>100</v>
       </c>
@@ -1542,11 +1738,15 @@
         <v>0.25</v>
       </c>
       <c r="F38">
-        <f>_xll.BLACK.VALUE(B38,C38,D38,E38)</f>
-        <v>7.1712785170343807</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B38,C38,D38,E38)</f>
+        <v>7.1712785170344233</v>
+      </c>
+      <c r="G38" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B38, F38, D38, E38)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>100</v>
       </c>
@@ -1560,11 +1760,15 @@
         <v>0.25</v>
       </c>
       <c r="F39">
-        <f>_xll.BLACK.VALUE(B39,C39,D39,E39)</f>
-        <v>7.3699208777894114</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B39,C39,D39,E39)</f>
+        <v>7.3699208777893759</v>
+      </c>
+      <c r="G39" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B39, F39, D39, E39)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>100</v>
       </c>
@@ -1578,11 +1782,15 @@
         <v>0.25</v>
       </c>
       <c r="F40">
-        <f>_xll.BLACK.VALUE(B40,C40,D40,E40)</f>
-        <v>7.5685173078332326</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B40,C40,D40,E40)</f>
+        <v>7.568517307833261</v>
+      </c>
+      <c r="G40" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B40, F40, D40, E40)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>100</v>
       </c>
@@ -1596,11 +1804,15 @@
         <v>0.25</v>
       </c>
       <c r="F41">
-        <f>_xll.BLACK.VALUE(B41,C41,D41,E41)</f>
-        <v>7.7670665768501124</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B41,C41,D41,E41)</f>
+        <v>7.7670665768501834</v>
+      </c>
+      <c r="G41" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B41, F41, D41, E41)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>100</v>
       </c>
@@ -1614,11 +1826,15 @@
         <v>0.25</v>
       </c>
       <c r="F42">
-        <f>_xll.BLACK.VALUE(B42,C42,D42,E42)</f>
-        <v>7.965567455405818</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B42,C42,D42,E42)</f>
+        <v>7.9655674554058038</v>
+      </c>
+      <c r="G42" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B42, F42, D42, E42)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>100</v>
       </c>
@@ -1632,11 +1848,15 @@
         <v>0.25</v>
       </c>
       <c r="F43">
-        <f>_xll.BLACK.VALUE(B43,C43,D43,E43)</f>
-        <v>8.1640187149702825</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B43,C43,D43,E43)</f>
+        <v>8.1640187149702541</v>
+      </c>
+      <c r="G43" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B43, F43, D43, E43)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>100</v>
       </c>
@@ -1650,11 +1870,15 @@
         <v>0.25</v>
       </c>
       <c r="F44">
-        <f>_xll.BLACK.VALUE(B44,C44,D44,E44)</f>
-        <v>8.3624191279409104</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B44,C44,D44,E44)</f>
+        <v>8.3624191279409317</v>
+      </c>
+      <c r="G44" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B44, F44, D44, E44)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>100</v>
       </c>
@@ -1668,11 +1892,15 @@
         <v>0.25</v>
       </c>
       <c r="F45">
-        <f>_xll.BLACK.VALUE(B45,C45,D45,E45)</f>
-        <v>8.5607674676652721</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B45,C45,D45,E45)</f>
+        <v>8.5607674676652294</v>
+      </c>
+      <c r="G45" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B45, F45, D45, E45)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>100</v>
       </c>
@@ -1686,11 +1914,15 @@
         <v>0.25</v>
       </c>
       <c r="F46">
-        <f>_xll.BLACK.VALUE(B46,C46,D46,E46)</f>
-        <v>8.7590625084633444</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B46,C46,D46,E46)</f>
+        <v>8.7590625084633658</v>
+      </c>
+      <c r="G46" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B46, F46, D46, E46)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>100</v>
       </c>
@@ -1704,11 +1936,15 @@
         <v>0.25</v>
       </c>
       <c r="F47">
-        <f>_xll.BLACK.VALUE(B47,C47,D47,E47)</f>
-        <v>8.9573030256509867</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B47,C47,D47,E47)</f>
+        <v>8.957303025651008</v>
+      </c>
+      <c r="G47" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B47, F47, D47, E47)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>100</v>
       </c>
@@ -1722,11 +1958,15 @@
         <v>0.25</v>
       </c>
       <c r="F48">
-        <f>_xll.BLACK.VALUE(B48,C48,D48,E48)</f>
-        <v>9.15548779556201</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B48,C48,D48,E48)</f>
+        <v>9.1554877955620526</v>
+      </c>
+      <c r="G48" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B48, F48, D48, E48)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>100</v>
       </c>
@@ -1740,11 +1980,15 @@
         <v>0.25</v>
       </c>
       <c r="F49">
-        <f>_xll.BLACK.VALUE(B49,C49,D49,E49)</f>
+        <f>_xll.XLL.BLACK.VALUE(B49,C49,D49,E49)</f>
         <v>9.3536155955712417</v>
       </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B49, F49, D49, E49)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>100</v>
       </c>
@@ -1758,11 +2002,15 @@
         <v>0.25</v>
       </c>
       <c r="F50">
-        <f>_xll.BLACK.VALUE(B50,C50,D50,E50)</f>
+        <f>_xll.XLL.BLACK.VALUE(B50,C50,D50,E50)</f>
         <v>9.5516852041167795</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G50" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B50, F50, D50, E50)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>100</v>
       </c>
@@ -1776,11 +2024,15 @@
         <v>0.25</v>
       </c>
       <c r="F51">
-        <f>_xll.BLACK.VALUE(B51,C51,D51,E51)</f>
-        <v>9.7496954007228993</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B51,C51,D51,E51)</f>
+        <v>9.7496954007229277</v>
+      </c>
+      <c r="G51" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B51, F51, D51, E51)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>100</v>
       </c>
@@ -1794,11 +2046,15 @@
         <v>0.25</v>
       </c>
       <c r="F52">
-        <f>_xll.BLACK.VALUE(B52,C52,D52,E52)</f>
-        <v>9.9476449660226223</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B52,C52,D52,E52)</f>
+        <v>9.9476449660225796</v>
+      </c>
+      <c r="G52" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B52, F52, D52, E52)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>100</v>
       </c>
@@ -1812,11 +2068,15 @@
         <v>0.25</v>
       </c>
       <c r="F53">
-        <f>_xll.BLACK.VALUE(B53,C53,D53,E53)</f>
-        <v>10.145532681779798</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B53,C53,D53,E53)</f>
+        <v>10.145532681779791</v>
+      </c>
+      <c r="G53" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B53, F53, D53, E53)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>100</v>
       </c>
@@ -1830,11 +2090,15 @@
         <v>0.25</v>
       </c>
       <c r="F54">
-        <f>_xll.BLACK.VALUE(B54,C54,D54,E54)</f>
-        <v>10.343357330912184</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B54,C54,D54,E54)</f>
+        <v>10.343357330912227</v>
+      </c>
+      <c r="G54" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B54, F54, D54, E54)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>100</v>
       </c>
@@ -1848,11 +2112,15 @@
         <v>0.25</v>
       </c>
       <c r="F55">
-        <f>_xll.BLACK.VALUE(B55,C55,D55,E55)</f>
-        <v>10.541117697513698</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B55,C55,D55,E55)</f>
+        <v>10.541117697513663</v>
+      </c>
+      <c r="G55" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B55, F55, D55, E55)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>100</v>
       </c>
@@ -1866,11 +2134,15 @@
         <v>0.25</v>
       </c>
       <c r="F56">
-        <f>_xll.BLACK.VALUE(B56,C56,D56,E56)</f>
-        <v>10.738812566876362</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B56,C56,D56,E56)</f>
+        <v>10.738812566876348</v>
+      </c>
+      <c r="G56" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B56, F56, D56, E56)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>100</v>
       </c>
@@ -1884,11 +2156,15 @@
         <v>0.25</v>
       </c>
       <c r="F57">
-        <f>_xll.BLACK.VALUE(B57,C57,D57,E57)</f>
-        <v>10.936440725513407</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B57,C57,D57,E57)</f>
+        <v>10.936440725513435</v>
+      </c>
+      <c r="G57" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B57, F57, D57, E57)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>100</v>
       </c>
@@ -1902,11 +2178,15 @@
         <v>0.25</v>
       </c>
       <c r="F58">
-        <f>_xll.BLACK.VALUE(B58,C58,D58,E58)</f>
-        <v>11.134000961181329</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B58,C58,D58,E58)</f>
+        <v>11.134000961181286</v>
+      </c>
+      <c r="G58" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B58, F58, D58, E58)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>100</v>
       </c>
@@ -1920,11 +2200,15 @@
         <v>0.25</v>
       </c>
       <c r="F59">
-        <f>_xll.BLACK.VALUE(B59,C59,D59,E59)</f>
-        <v>11.331492062901788</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B59,C59,D59,E59)</f>
+        <v>11.331492062901823</v>
+      </c>
+      <c r="G59" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B59, F59, D59, E59)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>100</v>
       </c>
@@ -1938,11 +2222,15 @@
         <v>0.25</v>
       </c>
       <c r="F60">
-        <f>_xll.BLACK.VALUE(B60,C60,D60,E60)</f>
-        <v>11.528912820984672</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B60,C60,D60,E60)</f>
+        <v>11.528912820984694</v>
+      </c>
+      <c r="G60" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B60, F60, D60, E60)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>100</v>
       </c>
@@ -1956,11 +2244,15 @@
         <v>0.25</v>
       </c>
       <c r="F61">
-        <f>_xll.BLACK.VALUE(B61,C61,D61,E61)</f>
-        <v>11.7262620270496</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B61,C61,D61,E61)</f>
+        <v>11.726262027049636</v>
+      </c>
+      <c r="G61" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B61, F61, D61, E61)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>100</v>
       </c>
@@ -1974,11 +2266,15 @@
         <v>0.25</v>
       </c>
       <c r="F62">
-        <f>_xll.BLACK.VALUE(B62,C62,D62,E62)</f>
+        <f>_xll.XLL.BLACK.VALUE(B62,C62,D62,E62)</f>
         <v>11.923538474048499</v>
       </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G62" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B62, F62, D62, E62)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>100</v>
       </c>
@@ -1992,11 +2288,15 @@
         <v>0.25</v>
       </c>
       <c r="F63">
-        <f>_xll.BLACK.VALUE(B63,C63,D63,E63)</f>
-        <v>12.120740956287506</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B63,C63,D63,E63)</f>
+        <v>12.120740956287527</v>
+      </c>
+      <c r="G63" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B63, F63, D63, E63)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>100</v>
       </c>
@@ -2010,11 +2310,15 @@
         <v>0.25</v>
       </c>
       <c r="F64">
-        <f>_xll.BLACK.VALUE(B64,C64,D64,E64)</f>
-        <v>12.317868269449335</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B64,C64,D64,E64)</f>
+        <v>12.317868269449377</v>
+      </c>
+      <c r="G64" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B64, F64, D64, E64)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>100</v>
       </c>
@@ -2028,11 +2332,15 @@
         <v>0.25</v>
       </c>
       <c r="F65">
-        <f>_xll.BLACK.VALUE(B65,C65,D65,E65)</f>
-        <v>12.514919210615204</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B65,C65,D65,E65)</f>
+        <v>12.514919210615169</v>
+      </c>
+      <c r="G65" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B65, F65, D65, E65)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>100</v>
       </c>
@@ -2046,11 +2354,15 @@
         <v>0.25</v>
       </c>
       <c r="F66">
-        <f>_xll.BLACK.VALUE(B66,C66,D66,E66)</f>
-        <v>12.71189257828658</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B66,C66,D66,E66)</f>
+        <v>12.711892578286573</v>
+      </c>
+      <c r="G66" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B66, F66, D66, E66)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>100</v>
       </c>
@@ -2064,11 +2376,15 @@
         <v>0.25</v>
       </c>
       <c r="F67">
-        <f>_xll.BLACK.VALUE(B67,C67,D67,E67)</f>
+        <f>_xll.XLL.BLACK.VALUE(B67,C67,D67,E67)</f>
         <v>12.908787172407685</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G67" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B67, F67, D67, E67)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>100</v>
       </c>
@@ -2082,11 +2398,15 @@
         <v>0.25</v>
       </c>
       <c r="F68">
-        <f>_xll.BLACK.VALUE(B68,C68,D68,E68)</f>
-        <v>13.105601794387084</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B68,C68,D68,E68)</f>
+        <v>13.105601794387042</v>
+      </c>
+      <c r="G68" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B68, F68, D68, E68)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>100</v>
       </c>
@@ -2100,11 +2420,15 @@
         <v>0.25</v>
       </c>
       <c r="F69">
-        <f>_xll.BLACK.VALUE(B69,C69,D69,E69)</f>
-        <v>13.30233524711943</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B69,C69,D69,E69)</f>
+        <v>13.302335247119416</v>
+      </c>
+      <c r="G69" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B69, F69, D69, E69)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>100</v>
       </c>
@@ -2118,11 +2442,15 @@
         <v>0.25</v>
       </c>
       <c r="F70">
-        <f>_xll.BLACK.VALUE(B70,C70,D70,E70)</f>
-        <v>13.498986335007658</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B70,C70,D70,E70)</f>
+        <v>13.498986335007686</v>
+      </c>
+      <c r="G70" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B70, F70, D70, E70)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>100</v>
       </c>
@@ -2136,11 +2464,15 @@
         <v>0.25</v>
       </c>
       <c r="F71">
-        <f>_xll.BLACK.VALUE(B71,C71,D71,E71)</f>
-        <v>13.695553863984628</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B71,C71,D71,E71)</f>
+        <v>13.695553863984649</v>
+      </c>
+      <c r="G71" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B71, F71, D71, E71)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>100</v>
       </c>
@@ -2154,11 +2486,15 @@
         <v>0.25</v>
       </c>
       <c r="F72">
-        <f>_xll.BLACK.VALUE(B72,C72,D72,E72)</f>
-        <v>13.892036641534759</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B72,C72,D72,E72)</f>
+        <v>13.89203664153473</v>
+      </c>
+      <c r="G72" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B72, F72, D72, E72)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>100</v>
       </c>
@@ -2172,11 +2508,15 @@
         <v>0.25</v>
       </c>
       <c r="F73">
-        <f>_xll.BLACK.VALUE(B73,C73,D73,E73)</f>
-        <v>14.08843347671565</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B73,C73,D73,E73)</f>
+        <v>14.088433476715664</v>
+      </c>
+      <c r="G73" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B73, F73, D73, E73)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>100</v>
       </c>
@@ -2190,11 +2530,15 @@
         <v>0.25</v>
       </c>
       <c r="F74">
-        <f>_xll.BLACK.VALUE(B74,C74,D74,E74)</f>
-        <v>14.284743180180115</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B74,C74,D74,E74)</f>
+        <v>14.284743180180143</v>
+      </c>
+      <c r="G74" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B74, F74, D74, E74)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>100</v>
       </c>
@@ -2208,11 +2552,15 @@
         <v>0.25</v>
       </c>
       <c r="F75">
-        <f>_xll.BLACK.VALUE(B75,C75,D75,E75)</f>
-        <v>14.48096456419745</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B75,C75,D75,E75)</f>
+        <v>14.480964564197436</v>
+      </c>
+      <c r="G75" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B75, F75, D75, E75)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>100</v>
       </c>
@@ -2226,11 +2574,15 @@
         <v>0.25</v>
       </c>
       <c r="F76">
-        <f>_xll.BLACK.VALUE(B76,C76,D76,E76)</f>
+        <f>_xll.XLL.BLACK.VALUE(B76,C76,D76,E76)</f>
         <v>14.67709644267488</v>
       </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G76" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B76, F76, D76, E76)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>100</v>
       </c>
@@ -2244,11 +2596,15 @@
         <v>0.25</v>
       </c>
       <c r="F77">
-        <f>_xll.BLACK.VALUE(B77,C77,D77,E77)</f>
-        <v>14.873137631179389</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B77,C77,D77,E77)</f>
+        <v>14.873137631179432</v>
+      </c>
+      <c r="G77" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B77, F77, D77, E77)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>100</v>
       </c>
@@ -2262,11 +2618,15 @@
         <v>0.25</v>
       </c>
       <c r="F78">
-        <f>_xll.BLACK.VALUE(B78,C78,D78,E78)</f>
+        <f>_xll.XLL.BLACK.VALUE(B78,C78,D78,E78)</f>
         <v>15.069086946959104</v>
       </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G78" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B78, F78, D78, E78)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>100</v>
       </c>
@@ -2280,11 +2640,15 @@
         <v>0.25</v>
       </c>
       <c r="F79">
-        <f>_xll.BLACK.VALUE(B79,C79,D79,E79)</f>
+        <f>_xll.XLL.BLACK.VALUE(B79,C79,D79,E79)</f>
         <v>15.264943208964226</v>
       </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G79" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B79, F79, D79, E79)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>100</v>
       </c>
@@ -2298,11 +2662,15 @@
         <v>0.25</v>
       </c>
       <c r="F80">
-        <f>_xll.BLACK.VALUE(B80,C80,D80,E80)</f>
+        <f>_xll.XLL.BLACK.VALUE(B80,C80,D80,E80)</f>
         <v>15.460705237869021</v>
       </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G80" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B80, F80, D80, E80)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>100</v>
       </c>
@@ -2316,11 +2684,15 @@
         <v>0.25</v>
       </c>
       <c r="F81">
-        <f>_xll.BLACK.VALUE(B81,C81,D81,E81)</f>
-        <v>15.656371856092704</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B81,C81,D81,E81)</f>
+        <v>15.656371856092647</v>
+      </c>
+      <c r="G81" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B81, F81, D81, E81)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>100</v>
       </c>
@@ -2334,11 +2706,15 @@
         <v>0.25</v>
       </c>
       <c r="F82">
-        <f>_xll.BLACK.VALUE(B82,C82,D82,E82)</f>
-        <v>15.851941887820644</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B82,C82,D82,E82)</f>
+        <v>15.851941887820608</v>
+      </c>
+      <c r="G82" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B82, F82, D82, E82)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>100</v>
       </c>
@@ -2352,11 +2728,15 @@
         <v>0.25</v>
       </c>
       <c r="F83">
-        <f>_xll.BLACK.VALUE(B83,C83,D83,E83)</f>
-        <v>16.047414159025749</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B83,C83,D83,E83)</f>
+        <v>16.047414159025777</v>
+      </c>
+      <c r="G83" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B83, F83, D83, E83)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>100</v>
       </c>
@@ -2370,11 +2750,15 @@
         <v>0.25</v>
       </c>
       <c r="F84">
-        <f>_xll.BLACK.VALUE(B84,C84,D84,E84)</f>
-        <v>16.242787497489573</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B84,C84,D84,E84)</f>
+        <v>16.242787497489637</v>
+      </c>
+      <c r="G84" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B84, F84, D84, E84)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>100</v>
       </c>
@@ -2388,11 +2772,15 @@
         <v>0.25</v>
       </c>
       <c r="F85">
-        <f>_xll.BLACK.VALUE(B85,C85,D85,E85)</f>
-        <v>16.438060732823303</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B85,C85,D85,E85)</f>
+        <v>16.438060732823274</v>
+      </c>
+      <c r="G85" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B85, F85, D85, E85)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>100</v>
       </c>
@@ -2406,11 +2794,15 @@
         <v>0.25</v>
       </c>
       <c r="F86">
-        <f>_xll.BLACK.VALUE(B86,C86,D86,E86)</f>
-        <v>16.633232696488449</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B86,C86,D86,E86)</f>
+        <v>16.633232696488463</v>
+      </c>
+      <c r="G86" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B86, F86, D86, E86)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>100</v>
       </c>
@@ -2424,11 +2816,15 @@
         <v>0.25</v>
       </c>
       <c r="F87">
-        <f>_xll.BLACK.VALUE(B87,C87,D87,E87)</f>
-        <v>16.828302221818475</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B87,C87,D87,E87)</f>
+        <v>16.828302221818483</v>
+      </c>
+      <c r="G87" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B87, F87, D87, E87)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>100</v>
       </c>
@@ -2442,11 +2838,15 @@
         <v>0.25</v>
       </c>
       <c r="F88">
-        <f>_xll.BLACK.VALUE(B88,C88,D88,E88)</f>
-        <v>17.023268144039179</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B88,C88,D88,E88)</f>
+        <v>17.023268144039164</v>
+      </c>
+      <c r="G88" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B88, F88, D88, E88)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>100</v>
       </c>
@@ -2460,11 +2860,15 @@
         <v>0.25</v>
       </c>
       <c r="F89">
-        <f>_xll.BLACK.VALUE(B89,C89,D89,E89)</f>
-        <v>17.21812930028959</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B89,C89,D89,E89)</f>
+        <v>17.218129300289561</v>
+      </c>
+      <c r="G89" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B89, F89, D89, E89)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>100</v>
       </c>
@@ -2478,11 +2882,15 @@
         <v>0.25</v>
       </c>
       <c r="F90">
-        <f>_xll.BLACK.VALUE(B90,C90,D90,E90)</f>
-        <v>17.412884529642909</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B90,C90,D90,E90)</f>
+        <v>17.412884529642916</v>
+      </c>
+      <c r="G90" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B90, F90, D90, E90)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>100</v>
       </c>
@@ -2496,11 +2904,15 @@
         <v>0.25</v>
       </c>
       <c r="F91">
-        <f>_xll.BLACK.VALUE(B91,C91,D91,E91)</f>
-        <v>17.607532673127253</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B91,C91,D91,E91)</f>
+        <v>17.607532673127224</v>
+      </c>
+      <c r="G91" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B91, F91, D91, E91)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>100</v>
       </c>
@@ -2514,11 +2926,15 @@
         <v>0.25</v>
       </c>
       <c r="F92">
-        <f>_xll.BLACK.VALUE(B92,C92,D92,E92)</f>
+        <f>_xll.XLL.BLACK.VALUE(B92,C92,D92,E92)</f>
         <v>17.802072573745932</v>
       </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G92" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B92, F92, D92, E92)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>100</v>
       </c>
@@ -2532,11 +2948,15 @@
         <v>0.25</v>
       </c>
       <c r="F93">
-        <f>_xll.BLACK.VALUE(B93,C93,D93,E93)</f>
+        <f>_xll.XLL.BLACK.VALUE(B93,C93,D93,E93)</f>
         <v>17.996503076498541</v>
       </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G93" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B93, F93, D93, E93)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>100</v>
       </c>
@@ -2550,11 +2970,15 @@
         <v>0.25</v>
       </c>
       <c r="F94">
-        <f>_xll.BLACK.VALUE(B94,C94,D94,E94)</f>
-        <v>18.190823028401155</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B94,C94,D94,E94)</f>
+        <v>18.190823028401184</v>
+      </c>
+      <c r="G94" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B94, F94, D94, E94)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>100</v>
       </c>
@@ -2568,11 +2992,15 @@
         <v>0.25</v>
       </c>
       <c r="F95">
-        <f>_xll.BLACK.VALUE(B95,C95,D95,E95)</f>
+        <f>_xll.XLL.BLACK.VALUE(B95,C95,D95,E95)</f>
         <v>18.385031278506986</v>
       </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G95" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B95, F95, D95, E95)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>100</v>
       </c>
@@ -2586,11 +3014,15 @@
         <v>0.25</v>
       </c>
       <c r="F96">
-        <f>_xll.BLACK.VALUE(B96,C96,D96,E96)</f>
+        <f>_xll.XLL.BLACK.VALUE(B96,C96,D96,E96)</f>
         <v>18.57912667792661</v>
       </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G96" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B96, F96, D96, E96)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>100</v>
       </c>
@@ -2604,11 +3036,15 @@
         <v>0.25</v>
       </c>
       <c r="F97">
-        <f>_xll.BLACK.VALUE(B97,C97,D97,E97)</f>
-        <v>18.77310807984847</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B97,C97,D97,E97)</f>
+        <v>18.773108079848484</v>
+      </c>
+      <c r="G97" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B97, F97, D97, E97)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>100</v>
       </c>
@@ -2622,11 +3058,15 @@
         <v>0.25</v>
       </c>
       <c r="F98">
-        <f>_xll.BLACK.VALUE(B98,C98,D98,E98)</f>
-        <v>18.966974339559158</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B98,C98,D98,E98)</f>
+        <v>18.966974339559165</v>
+      </c>
+      <c r="G98" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B98, F98, D98, E98)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>100</v>
       </c>
@@ -2640,11 +3080,15 @@
         <v>0.25</v>
       </c>
       <c r="F99">
-        <f>_xll.BLACK.VALUE(B99,C99,D99,E99)</f>
+        <f>_xll.XLL.BLACK.VALUE(B99,C99,D99,E99)</f>
         <v>19.160724314463522</v>
       </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G99" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B99, F99, D99, E99)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>100</v>
       </c>
@@ -2658,11 +3102,15 @@
         <v>0.25</v>
       </c>
       <c r="F100">
-        <f>_xll.BLACK.VALUE(B100,C100,D100,E100)</f>
-        <v>19.354356864104844</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B100,C100,D100,E100)</f>
+        <v>19.354356864104886</v>
+      </c>
+      <c r="G100" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B100, F100, D100, E100)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>100</v>
       </c>
@@ -2676,11 +3124,15 @@
         <v>0.25</v>
       </c>
       <c r="F101">
-        <f>_xll.BLACK.VALUE(B101,C101,D101,E101)</f>
-        <v>19.547870850185191</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B101,C101,D101,E101)</f>
+        <v>19.54787085018512</v>
+      </c>
+      <c r="G101" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B101, F101, D101, E101)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>100</v>
       </c>
@@ -2694,11 +3146,15 @@
         <v>0.25</v>
       </c>
       <c r="F102">
-        <f>_xll.BLACK.VALUE(B102,C102,D102,E102)</f>
-        <v>19.741265136584744</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B102,C102,D102,E102)</f>
+        <v>19.741265136584751</v>
+      </c>
+      <c r="G102" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B102, F102, D102, E102)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>100</v>
       </c>
@@ -2712,11 +3168,15 @@
         <v>0.25</v>
       </c>
       <c r="F103">
-        <f>_xll.BLACK.VALUE(B103,C103,D103,E103)</f>
-        <v>19.934538589382726</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B103,C103,D103,E103)</f>
+        <v>19.934538589382733</v>
+      </c>
+      <c r="G103" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B103, F103, D103, E103)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>100</v>
       </c>
@@ -2730,11 +3190,15 @@
         <v>0.25</v>
       </c>
       <c r="F104">
-        <f>_xll.BLACK.VALUE(B104,C104,D104,E104)</f>
-        <v>20.127690076876448</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B104,C104,D104,E104)</f>
+        <v>20.127690076876519</v>
+      </c>
+      <c r="G104" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B104, F104, D104, E104)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>100</v>
       </c>
@@ -2748,11 +3212,15 @@
         <v>0.25</v>
       </c>
       <c r="F105">
-        <f>_xll.BLACK.VALUE(B105,C105,D105,E105)</f>
+        <f>_xll.XLL.BLACK.VALUE(B105,C105,D105,E105)</f>
         <v>20.320718469601758</v>
       </c>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G105" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B105, F105, D105, E105)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>100</v>
       </c>
@@ -2766,11 +3234,15 @@
         <v>0.25</v>
       </c>
       <c r="F106">
-        <f>_xll.BLACK.VALUE(B106,C106,D106,E106)</f>
-        <v>20.513622640352082</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B106,C106,D106,E106)</f>
+        <v>20.513622640352096</v>
+      </c>
+      <c r="G106" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B106, F106, D106, E106)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>100</v>
       </c>
@@ -2784,11 +3256,15 @@
         <v>0.25</v>
       </c>
       <c r="F107">
-        <f>_xll.BLACK.VALUE(B107,C107,D107,E107)</f>
-        <v>20.706401464198862</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B107,C107,D107,E107)</f>
+        <v>20.706401464198905</v>
+      </c>
+      <c r="G107" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B107, F107, D107, E107)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>100</v>
       </c>
@@ -2802,11 +3278,15 @@
         <v>0.25</v>
       </c>
       <c r="F108">
-        <f>_xll.BLACK.VALUE(B108,C108,D108,E108)</f>
-        <v>20.899053818510822</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B108,C108,D108,E108)</f>
+        <v>20.899053818510808</v>
+      </c>
+      <c r="G108" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B108, F108, D108, E108)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>100</v>
       </c>
@@ -2820,11 +3300,15 @@
         <v>0.25</v>
       </c>
       <c r="F109">
-        <f>_xll.BLACK.VALUE(B109,C109,D109,E109)</f>
-        <v>21.091578582973199</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B109,C109,D109,E109)</f>
+        <v>21.091578582973213</v>
+      </c>
+      <c r="G109" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B109, F109, D109, E109)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>100</v>
       </c>
@@ -2838,11 +3322,15 @@
         <v>0.25</v>
       </c>
       <c r="F110">
-        <f>_xll.BLACK.VALUE(B110,C110,D110,E110)</f>
-        <v>21.283974639607891</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B110,C110,D110,E110)</f>
+        <v>21.283974639607898</v>
+      </c>
+      <c r="G110" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B110, F110, D110, E110)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>100</v>
       </c>
@@ -2856,11 +3344,15 @@
         <v>0.25</v>
       </c>
       <c r="F111">
-        <f>_xll.BLACK.VALUE(B111,C111,D111,E111)</f>
-        <v>21.47624087279236</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B111,C111,D111,E111)</f>
+        <v>21.476240872792324</v>
+      </c>
+      <c r="G111" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B111, F111, D111, E111)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>100</v>
       </c>
@@ -2874,11 +3366,15 @@
         <v>0.25</v>
       </c>
       <c r="F112">
-        <f>_xll.BLACK.VALUE(B112,C112,D112,E112)</f>
+        <f>_xll.XLL.BLACK.VALUE(B112,C112,D112,E112)</f>
         <v>21.668376169278972</v>
       </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G112" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B112, F112, D112, E112)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>100</v>
       </c>
@@ -2892,11 +3388,15 @@
         <v>0.25</v>
       </c>
       <c r="F113">
-        <f>_xll.BLACK.VALUE(B113,C113,D113,E113)</f>
-        <v>21.860379418214563</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B113,C113,D113,E113)</f>
+        <v>21.860379418214592</v>
+      </c>
+      <c r="G113" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B113, F113, D113, E113)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>100</v>
       </c>
@@ -2910,11 +3410,15 @@
         <v>0.25</v>
       </c>
       <c r="F114">
-        <f>_xll.BLACK.VALUE(B114,C114,D114,E114)</f>
-        <v>22.052249511159474</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B114,C114,D114,E114)</f>
+        <v>22.052249511159445</v>
+      </c>
+      <c r="G114" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B114, F114, D114, E114)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>100</v>
       </c>
@@ -2928,11 +3432,15 @@
         <v>0.25</v>
       </c>
       <c r="F115">
-        <f>_xll.BLACK.VALUE(B115,C115,D115,E115)</f>
-        <v>22.24398534210637</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B115,C115,D115,E115)</f>
+        <v>22.243985342106342</v>
+      </c>
+      <c r="G115" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B115, F115, D115, E115)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>100</v>
       </c>
@@ -2946,11 +3454,15 @@
         <v>0.25</v>
       </c>
       <c r="F116">
-        <f>_xll.BLACK.VALUE(B116,C116,D116,E116)</f>
+        <f>_xll.XLL.BLACK.VALUE(B116,C116,D116,E116)</f>
         <v>22.435585807499734</v>
       </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G116" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B116, F116, D116, E116)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>100</v>
       </c>
@@ -2964,11 +3476,15 @@
         <v>0.25</v>
       </c>
       <c r="F117">
-        <f>_xll.BLACK.VALUE(B117,C117,D117,E117)</f>
-        <v>22.62704980625459</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B117,C117,D117,E117)</f>
+        <v>22.627049806254611</v>
+      </c>
+      <c r="G117" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B117, F117, D117, E117)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>100</v>
       </c>
@@ -2982,11 +3498,15 @@
         <v>0.25</v>
       </c>
       <c r="F118">
-        <f>_xll.BLACK.VALUE(B118,C118,D118,E118)</f>
-        <v>22.818376239775489</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B118,C118,D118,E118)</f>
+        <v>22.818376239775475</v>
+      </c>
+      <c r="G118" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B118, F118, D118, E118)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>100</v>
       </c>
@@ -3000,11 +3520,15 @@
         <v>0.25</v>
       </c>
       <c r="F119">
-        <f>_xll.BLACK.VALUE(B119,C119,D119,E119)</f>
-        <v>23.009564011975044</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B119,C119,D119,E119)</f>
+        <v>23.009564011975037</v>
+      </c>
+      <c r="G119" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B119, F119, D119, E119)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>100</v>
       </c>
@@ -3018,11 +3542,15 @@
         <v>0.25</v>
       </c>
       <c r="F120">
-        <f>_xll.BLACK.VALUE(B120,C120,D120,E120)</f>
-        <v>23.20061202929304</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B120,C120,D120,E120)</f>
+        <v>23.200612029293083</v>
+      </c>
+      <c r="G120" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B120, F120, D120, E120)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>100</v>
       </c>
@@ -3036,11 +3564,15 @@
         <v>0.25</v>
       </c>
       <c r="F121">
-        <f>_xll.BLACK.VALUE(B121,C121,D121,E121)</f>
+        <f>_xll.XLL.BLACK.VALUE(B121,C121,D121,E121)</f>
         <v>23.391519200715024</v>
       </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G121" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B121, F121, D121, E121)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>100</v>
       </c>
@@ -3054,11 +3586,15 @@
         <v>0.25</v>
       </c>
       <c r="F122">
-        <f>_xll.BLACK.VALUE(B122,C122,D122,E122)</f>
-        <v>23.58228443779052</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B122,C122,D122,E122)</f>
+        <v>23.582284437790527</v>
+      </c>
+      <c r="G122" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B122, F122, D122, E122)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>100</v>
       </c>
@@ -3072,11 +3608,15 @@
         <v>0.25</v>
       </c>
       <c r="F123">
-        <f>_xll.BLACK.VALUE(B123,C123,D123,E123)</f>
-        <v>23.772906654651976</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B123,C123,D123,E123)</f>
+        <v>23.77290665465199</v>
+      </c>
+      <c r="G123" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B123, F123, D123, E123)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>100</v>
       </c>
@@ -3090,11 +3630,15 @@
         <v>0.25</v>
       </c>
       <c r="F124">
-        <f>_xll.BLACK.VALUE(B124,C124,D124,E124)</f>
-        <v>23.963384768033038</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B124,C124,D124,E124)</f>
+        <v>23.963384768033009</v>
+      </c>
+      <c r="G124" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B124, F124, D124, E124)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>100</v>
       </c>
@@ -3108,11 +3652,15 @@
         <v>0.25</v>
       </c>
       <c r="F125">
-        <f>_xll.BLACK.VALUE(B125,C125,D125,E125)</f>
+        <f>_xll.XLL.BLACK.VALUE(B125,C125,D125,E125)</f>
         <v>24.153717697286666</v>
       </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G125" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B125, F125, D125, E125)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>100</v>
       </c>
@@ -3126,11 +3674,15 @@
         <v>0.25</v>
       </c>
       <c r="F126">
-        <f>_xll.BLACK.VALUE(B126,C126,D126,E126)</f>
-        <v>24.343904364403841</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B126,C126,D126,E126)</f>
+        <v>24.343904364403855</v>
+      </c>
+      <c r="G126" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B126, F126, D126, E126)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>100</v>
       </c>
@@ -3144,11 +3696,15 @@
         <v>0.25</v>
       </c>
       <c r="F127">
-        <f>_xll.BLACK.VALUE(B127,C127,D127,E127)</f>
-        <v>24.533943694031393</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B127,C127,D127,E127)</f>
+        <v>24.533943694031407</v>
+      </c>
+      <c r="G127" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B127, F127, D127, E127)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>100</v>
       </c>
@@ -3162,11 +3718,15 @@
         <v>0.25</v>
       </c>
       <c r="F128">
-        <f>_xll.BLACK.VALUE(B128,C128,D128,E128)</f>
+        <f>_xll.XLL.BLACK.VALUE(B128,C128,D128,E128)</f>
         <v>24.723834613490283</v>
       </c>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G128" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B128, F128, D128, E128)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>100</v>
       </c>
@@ -3180,11 +3740,15 @@
         <v>0.25</v>
       </c>
       <c r="F129">
-        <f>_xll.BLACK.VALUE(B129,C129,D129,E129)</f>
-        <v>24.913576052793474</v>
-      </c>
-    </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B129,C129,D129,E129)</f>
+        <v>24.913576052793445</v>
+      </c>
+      <c r="G129" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B129, F129, D129, E129)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130">
         <v>100</v>
       </c>
@@ -3198,11 +3762,15 @@
         <v>0.25</v>
       </c>
       <c r="F130">
-        <f>_xll.BLACK.VALUE(B130,C130,D130,E130)</f>
-        <v>25.103166944663997</v>
-      </c>
-    </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B130,C130,D130,E130)</f>
+        <v>25.103166944664011</v>
+      </c>
+      <c r="G130" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B130, F130, D130, E130)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131">
         <v>100</v>
       </c>
@@ -3216,11 +3784,15 @@
         <v>0.25</v>
       </c>
       <c r="F131">
-        <f>_xll.BLACK.VALUE(B131,C131,D131,E131)</f>
-        <v>25.292606224552912</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B131,C131,D131,E131)</f>
+        <v>25.292606224552905</v>
+      </c>
+      <c r="G131" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B131, F131, D131, E131)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132">
         <v>100</v>
       </c>
@@ -3234,11 +3806,15 @@
         <v>0.25</v>
       </c>
       <c r="F132">
-        <f>_xll.BLACK.VALUE(B132,C132,D132,E132)</f>
-        <v>25.481892830656832</v>
-      </c>
-    </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B132,C132,D132,E132)</f>
+        <v>25.481892830656804</v>
+      </c>
+      <c r="G132" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B132, F132, D132, E132)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B133">
         <v>100</v>
       </c>
@@ -3252,11 +3828,15 @@
         <v>0.25</v>
       </c>
       <c r="F133">
-        <f>_xll.BLACK.VALUE(B133,C133,D133,E133)</f>
-        <v>25.671025703935697</v>
-      </c>
-    </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B133,C133,D133,E133)</f>
+        <v>25.67102570393574</v>
+      </c>
+      <c r="G133" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B133, F133, D133, E133)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134">
         <v>100</v>
       </c>
@@ -3270,11 +3850,15 @@
         <v>0.25</v>
       </c>
       <c r="F134">
-        <f>_xll.BLACK.VALUE(B134,C134,D134,E134)</f>
-        <v>25.86000378813074</v>
-      </c>
-    </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B134,C134,D134,E134)</f>
+        <v>25.860003788130697</v>
+      </c>
+      <c r="G134" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B134, F134, D134, E134)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135">
         <v>100</v>
       </c>
@@ -3288,11 +3872,15 @@
         <v>0.25</v>
       </c>
       <c r="F135">
-        <f>_xll.BLACK.VALUE(B135,C135,D135,E135)</f>
+        <f>_xll.XLL.BLACK.VALUE(B135,C135,D135,E135)</f>
         <v>26.048826029781267</v>
       </c>
-    </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G135" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B135, F135, D135, E135)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136">
         <v>100</v>
       </c>
@@ -3306,11 +3894,15 @@
         <v>0.25</v>
       </c>
       <c r="F136">
-        <f>_xll.BLACK.VALUE(B136,C136,D136,E136)</f>
-        <v>26.237491378242936</v>
-      </c>
-    </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B136,C136,D136,E136)</f>
+        <v>26.237491378242964</v>
+      </c>
+      <c r="G136" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B136, F136, D136, E136)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137">
         <v>100</v>
       </c>
@@ -3324,11 +3916,15 @@
         <v>0.25</v>
       </c>
       <c r="F137">
-        <f>_xll.BLACK.VALUE(B137,C137,D137,E137)</f>
-        <v>26.425998785704635</v>
-      </c>
-    </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B137,C137,D137,E137)</f>
+        <v>26.425998785704593</v>
+      </c>
+      <c r="G137" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B137, F137, D137, E137)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>100</v>
       </c>
@@ -3342,11 +3938,15 @@
         <v>0.25</v>
       </c>
       <c r="F138">
-        <f>_xll.BLACK.VALUE(B138,C138,D138,E138)</f>
-        <v>26.61434720720564</v>
-      </c>
-    </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B138,C138,D138,E138)</f>
+        <v>26.614347207205611</v>
+      </c>
+      <c r="G138" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B138, F138, D138, E138)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139">
         <v>100</v>
       </c>
@@ -3360,11 +3960,15 @@
         <v>0.25</v>
       </c>
       <c r="F139">
-        <f>_xll.BLACK.VALUE(B139,C139,D139,E139)</f>
-        <v>26.802535600653243</v>
-      </c>
-    </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B139,C139,D139,E139)</f>
+        <v>26.802535600653272</v>
+      </c>
+      <c r="G139" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B139, F139, D139, E139)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>100</v>
       </c>
@@ -3378,11 +3982,15 @@
         <v>0.25</v>
       </c>
       <c r="F140">
-        <f>_xll.BLACK.VALUE(B140,C140,D140,E140)</f>
-        <v>26.990562926839658</v>
-      </c>
-    </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B140,C140,D140,E140)</f>
+        <v>26.990562926839672</v>
+      </c>
+      <c r="G140" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B140, F140, D140, E140)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141">
         <v>100</v>
       </c>
@@ -3396,11 +4004,15 @@
         <v>0.25</v>
       </c>
       <c r="F141">
-        <f>_xll.BLACK.VALUE(B141,C141,D141,E141)</f>
+        <f>_xll.XLL.BLACK.VALUE(B141,C141,D141,E141)</f>
         <v>27.178428149458895</v>
       </c>
-    </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G141" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B141, F141, D141, E141)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142">
         <v>100</v>
       </c>
@@ -3414,11 +4026,15 @@
         <v>0.25</v>
       </c>
       <c r="F142">
-        <f>_xll.BLACK.VALUE(B142,C142,D142,E142)</f>
-        <v>27.366130235123791</v>
-      </c>
-    </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B142,C142,D142,E142)</f>
+        <v>27.366130235123819</v>
+      </c>
+      <c r="G142" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B142, F142, D142, E142)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>100</v>
       </c>
@@ -3432,11 +4048,15 @@
         <v>0.25</v>
       </c>
       <c r="F143">
-        <f>_xll.BLACK.VALUE(B143,C143,D143,E143)</f>
-        <v>27.553668153382958</v>
-      </c>
-    </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B143,C143,D143,E143)</f>
+        <v>27.553668153382986</v>
+      </c>
+      <c r="G143" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B143, F143, D143, E143)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>100</v>
       </c>
@@ -3450,11 +4070,15 @@
         <v>0.25</v>
       </c>
       <c r="F144">
-        <f>_xll.BLACK.VALUE(B144,C144,D144,E144)</f>
-        <v>27.741040876737458</v>
-      </c>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B144,C144,D144,E144)</f>
+        <v>27.741040876737429</v>
+      </c>
+      <c r="G144" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B144, F144, D144, E144)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B145">
         <v>100</v>
       </c>
@@ -3468,11 +4092,15 @@
         <v>0.25</v>
       </c>
       <c r="F145">
-        <f>_xll.BLACK.VALUE(B145,C145,D145,E145)</f>
-        <v>27.92824738065724</v>
-      </c>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B145,C145,D145,E145)</f>
+        <v>27.928247380657268</v>
+      </c>
+      <c r="G145" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B145, F145, D145, E145)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146">
         <v>100</v>
       </c>
@@ -3486,11 +4114,15 @@
         <v>0.25</v>
       </c>
       <c r="F146">
-        <f>_xll.BLACK.VALUE(B146,C146,D146,E146)</f>
-        <v>28.115286643598211</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B146,C146,D146,E146)</f>
+        <v>28.115286643598239</v>
+      </c>
+      <c r="G146" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B146, F146, D146, E146)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147">
         <v>100</v>
       </c>
@@ -3504,11 +4136,15 @@
         <v>0.25</v>
       </c>
       <c r="F147">
-        <f>_xll.BLACK.VALUE(B147,C147,D147,E147)</f>
+        <f>_xll.XLL.BLACK.VALUE(B147,C147,D147,E147)</f>
         <v>28.302157647018383</v>
       </c>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G147" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B147, F147, D147, E147)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148">
         <v>100</v>
       </c>
@@ -3522,11 +4158,15 @@
         <v>0.25</v>
       </c>
       <c r="F148">
-        <f>_xll.BLACK.VALUE(B148,C148,D148,E148)</f>
+        <f>_xll.XLL.BLACK.VALUE(B148,C148,D148,E148)</f>
         <v>28.488859375394156</v>
       </c>
-    </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G148" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B148, F148, D148, E148)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149">
         <v>100</v>
       </c>
@@ -3540,11 +4180,15 @@
         <v>0.25</v>
       </c>
       <c r="F149">
-        <f>_xll.BLACK.VALUE(B149,C149,D149,E149)</f>
+        <f>_xll.XLL.BLACK.VALUE(B149,C149,D149,E149)</f>
         <v>28.675390816236984</v>
       </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G149" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B149, F149, D149, E149)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150">
         <v>100</v>
       </c>
@@ -3558,11 +4202,15 @@
         <v>0.25</v>
       </c>
       <c r="F150">
-        <f>_xll.BLACK.VALUE(B150,C150,D150,E150)</f>
-        <v>28.861750960109305</v>
-      </c>
-    </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B150,C150,D150,E150)</f>
+        <v>28.861750960109362</v>
+      </c>
+      <c r="G150" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B150, F150, D150, E150)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151">
         <v>100</v>
       </c>
@@ -3576,11 +4224,15 @@
         <v>0.25</v>
       </c>
       <c r="F151">
-        <f>_xll.BLACK.VALUE(B151,C151,D151,E151)</f>
+        <f>_xll.XLL.BLACK.VALUE(B151,C151,D151,E151)</f>
         <v>29.047938800640964</v>
       </c>
-    </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G151" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B151, F151, D151, E151)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152">
         <v>100</v>
       </c>
@@ -3594,11 +4246,15 @@
         <v>0.25</v>
       </c>
       <c r="F152">
-        <f>_xll.BLACK.VALUE(B152,C152,D152,E152)</f>
-        <v>29.233953334544744</v>
-      </c>
-    </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B152,C152,D152,E152)</f>
+        <v>29.233953334544751</v>
+      </c>
+      <c r="G152" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B152, F152, D152, E152)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153">
         <v>100</v>
       </c>
@@ -3612,11 +4268,15 @@
         <v>0.25</v>
       </c>
       <c r="F153">
-        <f>_xll.BLACK.VALUE(B153,C153,D153,E153)</f>
-        <v>29.419793561632844</v>
-      </c>
-    </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B153,C153,D153,E153)</f>
+        <v>29.4197935616329</v>
+      </c>
+      <c r="G153" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B153, F153, D153, E153)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B154">
         <v>100</v>
       </c>
@@ -3630,11 +4290,15 @@
         <v>0.25</v>
       </c>
       <c r="F154">
-        <f>_xll.BLACK.VALUE(B154,C154,D154,E154)</f>
-        <v>29.605458484832582</v>
-      </c>
-    </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B154,C154,D154,E154)</f>
+        <v>29.605458484832553</v>
+      </c>
+      <c r="G154" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B154, F154, D154, E154)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B155">
         <v>100</v>
       </c>
@@ -3648,11 +4312,15 @@
         <v>0.25</v>
       </c>
       <c r="F155">
-        <f>_xll.BLACK.VALUE(B155,C155,D155,E155)</f>
-        <v>29.790947110201721</v>
-      </c>
-    </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B155,C155,D155,E155)</f>
+        <v>29.790947110201735</v>
+      </c>
+      <c r="G155" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B155, F155, D155, E155)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B156">
         <v>100</v>
       </c>
@@ -3666,11 +4334,15 @@
         <v>0.25</v>
       </c>
       <c r="F156">
-        <f>_xll.BLACK.VALUE(B156,C156,D156,E156)</f>
-        <v>29.976258446944854</v>
-      </c>
-    </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B156,C156,D156,E156)</f>
+        <v>29.976258446944875</v>
+      </c>
+      <c r="G156" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B156, F156, D156, E156)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157">
         <v>100</v>
       </c>
@@ -3684,11 +4356,15 @@
         <v>0.25</v>
       </c>
       <c r="F157">
-        <f>_xll.BLACK.VALUE(B157,C157,D157,E157)</f>
+        <f>_xll.XLL.BLACK.VALUE(B157,C157,D157,E157)</f>
         <v>30.161391507428448</v>
       </c>
-    </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G157" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B157, F157, D157, E157)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158">
         <v>100</v>
       </c>
@@ -3702,11 +4378,15 @@
         <v>0.25</v>
       </c>
       <c r="F158">
-        <f>_xll.BLACK.VALUE(B158,C158,D158,E158)</f>
-        <v>30.346345307196458</v>
-      </c>
-    </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B158,C158,D158,E158)</f>
+        <v>30.346345307196465</v>
+      </c>
+      <c r="G158" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B158, F158, D158, E158)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159">
         <v>100</v>
       </c>
@@ -3720,11 +4400,15 @@
         <v>0.25</v>
       </c>
       <c r="F159">
-        <f>_xll.BLACK.VALUE(B159,C159,D159,E159)</f>
-        <v>30.531118864985835</v>
-      </c>
-    </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B159,C159,D159,E159)</f>
+        <v>30.531118864985849</v>
+      </c>
+      <c r="G159" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B159, F159, D159, E159)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B160">
         <v>100</v>
       </c>
@@ -3738,11 +4422,15 @@
         <v>0.25</v>
       </c>
       <c r="F160">
-        <f>_xll.BLACK.VALUE(B160,C160,D160,E160)</f>
-        <v>30.715711202741687</v>
-      </c>
-    </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B160,C160,D160,E160)</f>
+        <v>30.715711202741659</v>
+      </c>
+      <c r="G160" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B160, F160, D160, E160)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B161">
         <v>100</v>
       </c>
@@ -3756,11 +4444,15 @@
         <v>0.25</v>
       </c>
       <c r="F161">
-        <f>_xll.BLACK.VALUE(B161,C161,D161,E161)</f>
-        <v>30.900121345632357</v>
-      </c>
-    </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B161,C161,D161,E161)</f>
+        <v>30.900121345632336</v>
+      </c>
+      <c r="G161" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B161, F161, D161, E161)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B162">
         <v>100</v>
       </c>
@@ -3774,11 +4466,15 @@
         <v>0.25</v>
       </c>
       <c r="F162">
-        <f>_xll.BLACK.VALUE(B162,C162,D162,E162)</f>
-        <v>31.084348322064812</v>
-      </c>
-    </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B162,C162,D162,E162)</f>
+        <v>31.084348322064841</v>
+      </c>
+      <c r="G162" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B162, F162, D162, E162)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B163">
         <v>100</v>
       </c>
@@ -3792,11 +4488,15 @@
         <v>0.25</v>
       </c>
       <c r="F163">
-        <f>_xll.BLACK.VALUE(B163,C163,D163,E163)</f>
-        <v>31.268391163699533</v>
-      </c>
-    </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B163,C163,D163,E163)</f>
+        <v>31.268391163699555</v>
+      </c>
+      <c r="G163" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B163, F163, D163, E163)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164">
         <v>100</v>
       </c>
@@ -3810,11 +4510,15 @@
         <v>0.25</v>
       </c>
       <c r="F164">
-        <f>_xll.BLACK.VALUE(B164,C164,D164,E164)</f>
+        <f>_xll.XLL.BLACK.VALUE(B164,C164,D164,E164)</f>
         <v>31.452248905465247</v>
       </c>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G164" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B164, F164, D164, E164)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B165">
         <v>100</v>
       </c>
@@ -3828,11 +4532,15 @@
         <v>0.25</v>
       </c>
       <c r="F165">
-        <f>_xll.BLACK.VALUE(B165,C165,D165,E165)</f>
+        <f>_xll.XLL.BLACK.VALUE(B165,C165,D165,E165)</f>
         <v>31.635920585573935</v>
       </c>
-    </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G165" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B165, F165, D165, E165)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B166">
         <v>100</v>
       </c>
@@ -3846,11 +4554,15 @@
         <v>0.25</v>
       </c>
       <c r="F166">
-        <f>_xll.BLACK.VALUE(B166,C166,D166,E166)</f>
-        <v>31.819405245535457</v>
-      </c>
-    </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B166,C166,D166,E166)</f>
+        <v>31.819405245535478</v>
+      </c>
+      <c r="G166" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B166, F166, D166, E166)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B167">
         <v>100</v>
       </c>
@@ -3864,11 +4576,15 @@
         <v>0.25</v>
       </c>
       <c r="F167">
-        <f>_xll.BLACK.VALUE(B167,C167,D167,E167)</f>
-        <v>32.002701930172293</v>
-      </c>
-    </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B167,C167,D167,E167)</f>
+        <v>32.002701930172272</v>
+      </c>
+      <c r="G167" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B167, F167, D167, E167)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B168">
         <v>100</v>
       </c>
@@ -3882,11 +4598,15 @@
         <v>0.25</v>
       </c>
       <c r="F168">
-        <f>_xll.BLACK.VALUE(B168,C168,D168,E168)</f>
+        <f>_xll.XLL.BLACK.VALUE(B168,C168,D168,E168)</f>
         <v>32.185809687633764</v>
       </c>
-    </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G168" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B168, F168, D168, E168)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B169">
         <v>100</v>
       </c>
@@ -3900,11 +4620,15 @@
         <v>0.25</v>
       </c>
       <c r="F169">
-        <f>_xll.BLACK.VALUE(B169,C169,D169,E169)</f>
+        <f>_xll.XLL.BLACK.VALUE(B169,C169,D169,E169)</f>
         <v>32.368727569410801</v>
       </c>
-    </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G169" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B169, F169, D169, E169)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B170">
         <v>100</v>
       </c>
@@ -3918,11 +4642,15 @@
         <v>0.25</v>
       </c>
       <c r="F170">
-        <f>_xll.BLACK.VALUE(B170,C170,D170,E170)</f>
-        <v>32.551454630350037</v>
-      </c>
-    </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B170,C170,D170,E170)</f>
+        <v>32.551454630350094</v>
+      </c>
+      <c r="G170" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B170, F170, D170, E170)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B171">
         <v>100</v>
       </c>
@@ -3936,11 +4664,15 @@
         <v>0.25</v>
       </c>
       <c r="F171">
-        <f>_xll.BLACK.VALUE(B171,C171,D171,E171)</f>
+        <f>_xll.XLL.BLACK.VALUE(B171,C171,D171,E171)</f>
         <v>32.733989928668279</v>
       </c>
-    </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G171" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B171, F171, D171, E171)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B172">
         <v>100</v>
       </c>
@@ -3954,11 +4686,15 @@
         <v>0.25</v>
       </c>
       <c r="F172">
-        <f>_xll.BLACK.VALUE(B172,C172,D172,E172)</f>
+        <f>_xll.XLL.BLACK.VALUE(B172,C172,D172,E172)</f>
         <v>32.916332525966084</v>
       </c>
-    </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G172" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B172, F172, D172, E172)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B173">
         <v>100</v>
       </c>
@@ -3972,11 +4708,15 @@
         <v>0.25</v>
       </c>
       <c r="F173">
-        <f>_xll.BLACK.VALUE(B173,C173,D173,E173)</f>
-        <v>33.098481487242481</v>
-      </c>
-    </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B173,C173,D173,E173)</f>
+        <v>33.098481487242509</v>
+      </c>
+      <c r="G173" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B173, F173, D173, E173)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B174">
         <v>100</v>
       </c>
@@ -3990,11 +4730,15 @@
         <v>0.25</v>
       </c>
       <c r="F174">
-        <f>_xll.BLACK.VALUE(B174,C174,D174,E174)</f>
+        <f>_xll.XLL.BLACK.VALUE(B174,C174,D174,E174)</f>
         <v>33.28043588090847</v>
       </c>
-    </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G174" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B174, F174, D174, E174)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B175">
         <v>100</v>
       </c>
@@ -4008,11 +4752,15 @@
         <v>0.25</v>
       </c>
       <c r="F175">
-        <f>_xll.BLACK.VALUE(B175,C175,D175,E175)</f>
+        <f>_xll.XLL.BLACK.VALUE(B175,C175,D175,E175)</f>
         <v>33.462194778800864</v>
       </c>
-    </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G175" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B175, F175, D175, E175)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B176">
         <v>100</v>
       </c>
@@ -4026,11 +4774,15 @@
         <v>0.25</v>
       </c>
       <c r="F176">
-        <f>_xll.BLACK.VALUE(B176,C176,D176,E176)</f>
-        <v>33.643757256196153</v>
-      </c>
-    </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B176,C176,D176,E176)</f>
+        <v>33.643757256196189</v>
+      </c>
+      <c r="G176" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B176, F176, D176, E176)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B177">
         <v>100</v>
       </c>
@@ -4044,11 +4796,15 @@
         <v>0.25</v>
       </c>
       <c r="F177">
-        <f>_xll.BLACK.VALUE(B177,C177,D177,E177)</f>
-        <v>33.825122391824181</v>
-      </c>
-    </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B177,C177,D177,E177)</f>
+        <v>33.825122391824152</v>
+      </c>
+      <c r="G177" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B177, F177, D177, E177)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>100</v>
       </c>
@@ -4062,11 +4818,15 @@
         <v>0.25</v>
       </c>
       <c r="F178">
-        <f>_xll.BLACK.VALUE(B178,C178,D178,E178)</f>
+        <f>_xll.XLL.BLACK.VALUE(B178,C178,D178,E178)</f>
         <v>34.006289267881272</v>
       </c>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G178" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B178, F178, D178, E178)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B179">
         <v>100</v>
       </c>
@@ -4080,11 +4840,15 @@
         <v>0.25</v>
       </c>
       <c r="F179">
-        <f>_xll.BLACK.VALUE(B179,C179,D179,E179)</f>
-        <v>34.187256970044139</v>
-      </c>
-    </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B179,C179,D179,E179)</f>
+        <v>34.18725697004416</v>
+      </c>
+      <c r="G179" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B179, F179, D179, E179)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>100</v>
       </c>
@@ -4098,11 +4862,15 @@
         <v>0.25</v>
       </c>
       <c r="F180">
-        <f>_xll.BLACK.VALUE(B180,C180,D180,E180)</f>
-        <v>34.368024587483028</v>
-      </c>
-    </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B180,C180,D180,E180)</f>
+        <v>34.368024587483042</v>
+      </c>
+      <c r="G180" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B180, F180, D180, E180)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B181">
         <v>100</v>
       </c>
@@ -4116,11 +4884,15 @@
         <v>0.25</v>
       </c>
       <c r="F181">
-        <f>_xll.BLACK.VALUE(B181,C181,D181,E181)</f>
+        <f>_xll.XLL.BLACK.VALUE(B181,C181,D181,E181)</f>
         <v>34.548591212874747</v>
       </c>
-    </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G181" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B181, F181, D181, E181)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>100</v>
       </c>
@@ -4134,11 +4906,15 @@
         <v>0.25</v>
       </c>
       <c r="F182">
-        <f>_xll.BLACK.VALUE(B182,C182,D182,E182)</f>
-        <v>34.728955942415979</v>
-      </c>
-    </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B182,C182,D182,E182)</f>
+        <v>34.728955942415986</v>
+      </c>
+      <c r="G182" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B182, F182, D182, E182)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B183">
         <v>100</v>
       </c>
@@ -4152,11 +4928,15 @@
         <v>0.25</v>
       </c>
       <c r="F183">
-        <f>_xll.BLACK.VALUE(B183,C183,D183,E183)</f>
-        <v>34.90911787583633</v>
-      </c>
-    </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B183,C183,D183,E183)</f>
+        <v>34.909117875836351</v>
+      </c>
+      <c r="G183" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B183, F183, D183, E183)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>100</v>
       </c>
@@ -4170,11 +4950,15 @@
         <v>0.25</v>
       </c>
       <c r="F184">
-        <f>_xll.BLACK.VALUE(B184,C184,D184,E184)</f>
-        <v>35.089076116411071</v>
-      </c>
-    </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B184,C184,D184,E184)</f>
+        <v>35.089076116411093</v>
+      </c>
+      <c r="G184" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B184, F184, D184, E184)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>100</v>
       </c>
@@ -4188,11 +4972,15 @@
         <v>0.25</v>
       </c>
       <c r="F185">
-        <f>_xll.BLACK.VALUE(B185,C185,D185,E185)</f>
-        <v>35.268829770974072</v>
-      </c>
-    </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B185,C185,D185,E185)</f>
+        <v>35.268829770974087</v>
+      </c>
+      <c r="G185" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B185, F185, D185, E185)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>100</v>
       </c>
@@ -4206,11 +4994,15 @@
         <v>0.25</v>
       </c>
       <c r="F186">
-        <f>_xll.BLACK.VALUE(B186,C186,D186,E186)</f>
-        <v>35.448377949930432</v>
-      </c>
-    </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B186,C186,D186,E186)</f>
+        <v>35.448377949930482</v>
+      </c>
+      <c r="G186" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B186, F186, D186, E186)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B187">
         <v>100</v>
       </c>
@@ -4224,11 +5016,15 @@
         <v>0.25</v>
       </c>
       <c r="F187">
-        <f>_xll.BLACK.VALUE(B187,C187,D187,E187)</f>
+        <f>_xll.XLL.BLACK.VALUE(B187,C187,D187,E187)</f>
         <v>35.627719767269191</v>
       </c>
-    </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G187" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B187, F187, D187, E187)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>100</v>
       </c>
@@ -4242,11 +5038,15 @@
         <v>0.25</v>
       </c>
       <c r="F188">
-        <f>_xll.BLACK.VALUE(B188,C188,D188,E188)</f>
-        <v>35.806854340575626</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B188,C188,D188,E188)</f>
+        <v>35.806854340575597</v>
+      </c>
+      <c r="G188" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B188, F188, D188, E188)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B189">
         <v>100</v>
       </c>
@@ -4260,11 +5060,15 @@
         <v>0.25</v>
       </c>
       <c r="F189">
-        <f>_xll.BLACK.VALUE(B189,C189,D189,E189)</f>
-        <v>35.985780791043759</v>
-      </c>
-    </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B189,C189,D189,E189)</f>
+        <v>35.985780791043787</v>
+      </c>
+      <c r="G189" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B189, F189, D189, E189)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B190">
         <v>100</v>
       </c>
@@ -4278,11 +5082,15 @@
         <v>0.25</v>
       </c>
       <c r="F190">
-        <f>_xll.BLACK.VALUE(B190,C190,D190,E190)</f>
-        <v>36.164498243488858</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B190,C190,D190,E190)</f>
+        <v>36.16449824348885</v>
+      </c>
+      <c r="G190" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B190, F190, D190, E190)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="191" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>100</v>
       </c>
@@ -4296,11 +5104,15 @@
         <v>0.25</v>
       </c>
       <c r="F191">
-        <f>_xll.BLACK.VALUE(B191,C191,D191,E191)</f>
+        <f>_xll.XLL.BLACK.VALUE(B191,C191,D191,E191)</f>
         <v>36.343005826359104</v>
       </c>
-    </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G191" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B191, F191, D191, E191)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>100</v>
       </c>
@@ -4314,11 +5126,15 @@
         <v>0.25</v>
       </c>
       <c r="F192">
-        <f>_xll.BLACK.VALUE(B192,C192,D192,E192)</f>
-        <v>36.521302671748153</v>
-      </c>
-    </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B192,C192,D192,E192)</f>
+        <v>36.521302671748181</v>
+      </c>
+      <c r="G192" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B192, F192, D192, E192)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B193">
         <v>100</v>
       </c>
@@ -4332,11 +5148,15 @@
         <v>0.25</v>
       </c>
       <c r="F193">
-        <f>_xll.BLACK.VALUE(B193,C193,D193,E193)</f>
+        <f>_xll.XLL.BLACK.VALUE(B193,C193,D193,E193)</f>
         <v>36.699387915406987</v>
       </c>
-    </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G193" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B193, F193, D193, E193)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194">
         <v>100</v>
       </c>
@@ -4350,11 +5170,15 @@
         <v>0.25</v>
       </c>
       <c r="F194">
-        <f>_xll.BLACK.VALUE(B194,C194,D194,E194)</f>
+        <f>_xll.XLL.BLACK.VALUE(B194,C194,D194,E194)</f>
         <v>36.877260696755485</v>
       </c>
-    </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G194" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B194, F194, D194, E194)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B195">
         <v>100</v>
       </c>
@@ -4368,11 +5192,15 @@
         <v>0.25</v>
       </c>
       <c r="F195">
-        <f>_xll.BLACK.VALUE(B195,C195,D195,E195)</f>
+        <f>_xll.XLL.BLACK.VALUE(B195,C195,D195,E195)</f>
         <v>37.054920158894596</v>
       </c>
-    </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G195" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B195, F195, D195, E195)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B196">
         <v>100</v>
       </c>
@@ -4386,11 +5214,15 @@
         <v>0.25</v>
       </c>
       <c r="F196">
-        <f>_xll.BLACK.VALUE(B196,C196,D196,E196)</f>
-        <v>37.232365448617713</v>
-      </c>
-    </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B196,C196,D196,E196)</f>
+        <v>37.23236544861777</v>
+      </c>
+      <c r="G196" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B196, F196, D196, E196)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B197">
         <v>100</v>
       </c>
@@ -4404,11 +5236,15 @@
         <v>0.25</v>
       </c>
       <c r="F197">
-        <f>_xll.BLACK.VALUE(B197,C197,D197,E197)</f>
+        <f>_xll.XLL.BLACK.VALUE(B197,C197,D197,E197)</f>
         <v>37.409595716422501</v>
       </c>
-    </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G197" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B197, F197, D197, E197)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B198">
         <v>100</v>
       </c>
@@ -4422,11 +5258,15 @@
         <v>0.25</v>
       </c>
       <c r="F198">
-        <f>_xll.BLACK.VALUE(B198,C198,D198,E198)</f>
+        <f>_xll.XLL.BLACK.VALUE(B198,C198,D198,E198)</f>
         <v>37.586610116521882</v>
       </c>
-    </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G198" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B198, F198, D198, E198)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B199">
         <v>100</v>
       </c>
@@ -4440,11 +5280,15 @@
         <v>0.25</v>
       </c>
       <c r="F199">
-        <f>_xll.BLACK.VALUE(B199,C199,D199,E199)</f>
-        <v>37.763407806855838</v>
-      </c>
-    </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B199,C199,D199,E199)</f>
+        <v>37.763407806855859</v>
+      </c>
+      <c r="G199" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B199, F199, D199, E199)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B200">
         <v>100</v>
       </c>
@@ -4458,11 +5302,15 @@
         <v>0.25</v>
       </c>
       <c r="F200">
-        <f>_xll.BLACK.VALUE(B200,C200,D200,E200)</f>
-        <v>37.939987949102459</v>
-      </c>
-    </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.25">
+        <f>_xll.XLL.BLACK.VALUE(B200,C200,D200,E200)</f>
+        <v>37.939987949102431</v>
+      </c>
+      <c r="G200" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B200, F200, D200, E200)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B201">
         <v>100</v>
       </c>
@@ -4476,11 +5324,15 @@
         <v>0.25</v>
       </c>
       <c r="F201">
-        <f>_xll.BLACK.VALUE(B201,C201,D201,E201)</f>
+        <f>_xll.XLL.BLACK.VALUE(B201,C201,D201,E201)</f>
         <v>38.116349708688858</v>
       </c>
-    </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G201" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B201, F201, D201, E201)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202">
         <v>100</v>
       </c>
@@ -4494,8 +5346,326 @@
         <v>0.25</v>
       </c>
       <c r="F202">
-        <f>_xll.BLACK.VALUE(B202,C202,D202,E202)</f>
-        <v>38.292492254802596</v>
+        <f>_xll.XLL.BLACK.VALUE(B202,C202,D202,E202)</f>
+        <v>38.292492254802625</v>
+      </c>
+      <c r="G202" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(B202, F202, D202, E202)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="E1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>0.3</v>
+      </c>
+      <c r="K1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <f>_xll.XLL.BIND(_xll.XLL.BLACK.VALUE,Forward,,Strike,Expiration)</f>
+        <v>-9.2559595921957428E+61</v>
+      </c>
+      <c r="F2">
+        <f>_xll.XLL.CONSTANT(C6)</f>
+        <v>-9.2559595921971129E+61</v>
+      </c>
+      <c r="G2">
+        <f>_xll.XLL.SUB(E2, F2)</f>
+        <v>-9.2559595921960168E+61</v>
+      </c>
+      <c r="I2">
+        <f>_xll.XLL.ROOT1D(G2)</f>
+        <v>-9.2559595922700693E+61</v>
+      </c>
+      <c r="J2">
+        <f>_xll.XLL.ROOT1D.INIT(I2, 0.3)</f>
+        <v>-9.2559595922700693E+61</v>
+      </c>
+      <c r="K2">
+        <f>_xll.XLL.ROOT1D.BRACKET(J2, K1)</f>
+        <v>-9.2559595922700693E+61</v>
+      </c>
+      <c r="M2">
+        <f>_xll.XLL.ROOT1D.STEP(K2, _xll.XLL.ROOT1D.STEP.SECANT())</f>
+        <v>-9.2559595922700693E+61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="J3">
+        <f t="array" ref="J3:J14">_xll.XLL.ROOT1D.X(J2)</f>
+        <v>0.3</v>
+      </c>
+      <c r="K3">
+        <f t="array" ref="K3:K14">_xll.XLL.ROOT1D.X(K2)</f>
+        <v>0.19992590000171551</v>
+      </c>
+      <c r="L3">
+        <f t="array" ref="L3:L14">_xll.XLL.ROOT1D.Y(K2)</f>
+        <v>-1.4762353511414972E-3</v>
+      </c>
+      <c r="M3">
+        <f t="array" ref="M3:M14">_xll.XLL.ROOT1D.X(M2)</f>
+        <v>0.19992590000171551</v>
+      </c>
+      <c r="N3">
+        <f t="array" ref="N3:N14">_xll.XLL.ROOT1D.Y(M2)</f>
+        <v>-1.4762353511414972E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>0.3</v>
+      </c>
+      <c r="K4">
+        <v>0.3</v>
+      </c>
+      <c r="L4">
+        <v>1.9907676429044656</v>
+      </c>
+      <c r="M4">
+        <v>0.23566152627740183</v>
+      </c>
+      <c r="N4">
+        <v>0.7102881711259954</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+      <c r="J5">
+        <v>0.3</v>
+      </c>
+      <c r="K5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5">
+        <v>0.3</v>
+      </c>
+      <c r="N5">
+        <v>1.9907676429044656</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <f>_xll.XLL.BLACK.VALUE(Forward, Volatility, Strike, Expiration)</f>
+        <v>3.987761167674492</v>
+      </c>
+      <c r="E6">
+        <f>_xll.XLL.CALL(E2,Volatility)</f>
+        <v>3.987761167674492</v>
+      </c>
+      <c r="F6">
+        <f>_xll.XLL.CALL(F2)</f>
+        <v>3.987761167674492</v>
+      </c>
+      <c r="G6">
+        <f>_xll.XLL.CALL(G2,Volatility)</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.3</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C7" t="e">
+        <f>_xll.XLL.BLACK.IMPLIED.VOLATILITY(Forward, Value, Strike, Expiration)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="J7">
+        <v>0.3</v>
+      </c>
+      <c r="K7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N7" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>0.3</v>
+      </c>
+      <c r="K8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N8" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>0.3</v>
+      </c>
+      <c r="K9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>0.3</v>
+      </c>
+      <c r="K10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N10" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>0.3</v>
+      </c>
+      <c r="K11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N11" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>0.3</v>
+      </c>
+      <c r="K12" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L12" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M12" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N12" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>0.3</v>
+      </c>
+      <c r="K13" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L13" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M13" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N13" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>0.3</v>
+      </c>
+      <c r="K14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N14" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>